<commit_message>
Silicon Croft - Planning nearly finished
</commit_message>
<xml_diff>
--- a/Graded Unit Project/Gantt Chart.xlsx
+++ b/Graded Unit Project/Gantt Chart.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{BD44F9EC-0DE4-4371-9300-9D3D547A64FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA1A6116-D958-4772-8FDD-F38BBC02DCC1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87180EA-7FC8-463D-9356-53047B064875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="27105" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="8265" windowWidth="43200" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -39,25 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="62">
-  <si>
-    <t>Task 3</t>
-  </si>
-  <si>
-    <t>Task 4</t>
-  </si>
-  <si>
-    <t>Task 5</t>
-  </si>
-  <si>
-    <t>Task 1</t>
-  </si>
-  <si>
-    <t>Task 2</t>
-  </si>
-  <si>
-    <t>Insert new rows ABOVE this one</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
   <si>
     <t>Project Start:</t>
   </si>
@@ -135,9 +117,6 @@
   </si>
   <si>
     <t>Enter Company Name in cell B2.</t>
-  </si>
-  <si>
-    <t>date</t>
   </si>
   <si>
     <t>Sample phase title block</t>
@@ -243,9 +222,6 @@
     <t>Decide Software Platform</t>
   </si>
   <si>
-    <t>Aquire Access to Hosting Provider</t>
-  </si>
-  <si>
     <t>Plan Website Prototype</t>
   </si>
   <si>
@@ -265,6 +241,57 @@
   </si>
   <si>
     <t>Install Server-Side Language</t>
+  </si>
+  <si>
+    <t>Decide Operating System</t>
+  </si>
+  <si>
+    <t>Aquire Access to Web Space</t>
+  </si>
+  <si>
+    <t>Plan Site Layout &amp; Pages</t>
+  </si>
+  <si>
+    <t>Create Site Map</t>
+  </si>
+  <si>
+    <t>Choose CMS Plugins</t>
+  </si>
+  <si>
+    <t>Explore Look &amp; Feel Options</t>
+  </si>
+  <si>
+    <t>Finalize Look &amp; Feel</t>
+  </si>
+  <si>
+    <t>Install And Configure Plugins</t>
+  </si>
+  <si>
+    <t>Populate Database With Assets</t>
+  </si>
+  <si>
+    <t>Create Any Required Assets</t>
+  </si>
+  <si>
+    <t>Create Pages From Site Map</t>
+  </si>
+  <si>
+    <t>Enforce Look &amp; Feel</t>
+  </si>
+  <si>
+    <t>Testing The Website</t>
+  </si>
+  <si>
+    <t>Bug-Fixing</t>
+  </si>
+  <si>
+    <t>Test Responsiveness</t>
+  </si>
+  <si>
+    <t>Test Navigation</t>
+  </si>
+  <si>
+    <t>Test Individual Pages</t>
   </si>
 </sst>
 </file>
@@ -458,7 +485,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -535,6 +562,18 @@
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -689,7 +728,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -936,12 +975,18 @@
     <xf numFmtId="170" fontId="9" fillId="10" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="15" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -951,11 +996,32 @@
     <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="15" fontId="9" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="2" xfId="12" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="14" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="9" fillId="14" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="15" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1523,165 +1589,112 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL37"/>
+  <dimension ref="A1:BL43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomLeft" activeCell="AF47" sqref="AF47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="58" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" style="5" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" customWidth="1"/>
     <col min="7" max="7" width="2.7109375" customWidth="1"/>
     <col min="8" max="8" width="6.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="64" width="2.5703125" customWidth="1"/>
+    <col min="9" max="29" width="6.7109375" customWidth="1"/>
+    <col min="30" max="64" width="5.7109375" customWidth="1"/>
     <col min="69" max="70" width="10.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="59" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B1" s="62" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
       <c r="E1" s="4"/>
       <c r="F1" s="47"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="81" t="s">
-        <v>17</v>
-      </c>
+      <c r="I1" s="81"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="58" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B2" s="63" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="82" t="s">
-        <v>22</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="I2" s="82"/>
     </row>
     <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B3" s="64" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="88" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="89"/>
-      <c r="E3" s="93">
+        <v>39</v>
+      </c>
+      <c r="C3" s="89" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="90"/>
+      <c r="E3" s="91">
         <v>44691</v>
       </c>
-      <c r="F3" s="93"/>
+      <c r="F3" s="91"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="88" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="89"/>
+        <v>30</v>
+      </c>
+      <c r="C4" s="89" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="90"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="90">
+      <c r="I4" s="92">
         <f>I5</f>
         <v>44690</v>
       </c>
-      <c r="J4" s="91"/>
-      <c r="K4" s="91"/>
-      <c r="L4" s="91"/>
-      <c r="M4" s="91"/>
-      <c r="N4" s="91"/>
-      <c r="O4" s="92"/>
-      <c r="P4" s="90">
+      <c r="J4" s="93"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="93"/>
+      <c r="M4" s="93"/>
+      <c r="N4" s="93"/>
+      <c r="O4" s="94"/>
+      <c r="P4" s="92">
         <f>P5</f>
         <v>44697</v>
       </c>
-      <c r="Q4" s="91"/>
-      <c r="R4" s="91"/>
-      <c r="S4" s="91"/>
-      <c r="T4" s="91"/>
-      <c r="U4" s="91"/>
-      <c r="V4" s="92"/>
-      <c r="W4" s="90">
+      <c r="Q4" s="93"/>
+      <c r="R4" s="93"/>
+      <c r="S4" s="93"/>
+      <c r="T4" s="93"/>
+      <c r="U4" s="93"/>
+      <c r="V4" s="94"/>
+      <c r="W4" s="92">
         <f>W5</f>
         <v>44704</v>
       </c>
-      <c r="X4" s="91"/>
-      <c r="Y4" s="91"/>
-      <c r="Z4" s="91"/>
-      <c r="AA4" s="91"/>
-      <c r="AB4" s="91"/>
-      <c r="AC4" s="92"/>
-      <c r="AD4" s="90">
-        <f>AD5</f>
-        <v>44711</v>
-      </c>
-      <c r="AE4" s="91"/>
-      <c r="AF4" s="91"/>
-      <c r="AG4" s="91"/>
-      <c r="AH4" s="91"/>
-      <c r="AI4" s="91"/>
-      <c r="AJ4" s="92"/>
-      <c r="AK4" s="90">
-        <f>AK5</f>
-        <v>44718</v>
-      </c>
-      <c r="AL4" s="91"/>
-      <c r="AM4" s="91"/>
-      <c r="AN4" s="91"/>
-      <c r="AO4" s="91"/>
-      <c r="AP4" s="91"/>
-      <c r="AQ4" s="92"/>
-      <c r="AR4" s="90">
-        <f>AR5</f>
-        <v>44725</v>
-      </c>
-      <c r="AS4" s="91"/>
-      <c r="AT4" s="91"/>
-      <c r="AU4" s="91"/>
-      <c r="AV4" s="91"/>
-      <c r="AW4" s="91"/>
-      <c r="AX4" s="92"/>
-      <c r="AY4" s="90">
-        <f>AY5</f>
-        <v>44732</v>
-      </c>
-      <c r="AZ4" s="91"/>
-      <c r="BA4" s="91"/>
-      <c r="BB4" s="91"/>
-      <c r="BC4" s="91"/>
-      <c r="BD4" s="91"/>
-      <c r="BE4" s="92"/>
-      <c r="BF4" s="90">
-        <f>BF5</f>
-        <v>44739</v>
-      </c>
-      <c r="BG4" s="91"/>
-      <c r="BH4" s="91"/>
-      <c r="BI4" s="91"/>
-      <c r="BJ4" s="91"/>
-      <c r="BK4" s="91"/>
-      <c r="BL4" s="92"/>
+      <c r="X4" s="93"/>
+      <c r="Y4" s="93"/>
+      <c r="Z4" s="93"/>
+      <c r="AA4" s="93"/>
+      <c r="AB4" s="93"/>
+      <c r="AC4" s="94"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B5" s="80"/>
       <c r="C5" s="80"/>
@@ -1698,7 +1711,7 @@
         <v>44691</v>
       </c>
       <c r="K5" s="10">
-        <f t="shared" ref="K5:AX5" si="0">J5+1</f>
+        <f t="shared" ref="K5:AC5" si="0">J5+1</f>
         <v>44692</v>
       </c>
       <c r="L5" s="10">
@@ -1773,398 +1786,118 @@
         <f t="shared" si="0"/>
         <v>44710</v>
       </c>
-      <c r="AD5" s="11">
-        <f>AC5+1</f>
-        <v>44711</v>
-      </c>
-      <c r="AE5" s="10">
-        <f>AD5+1</f>
-        <v>44712</v>
-      </c>
-      <c r="AF5" s="10">
-        <f t="shared" si="0"/>
-        <v>44713</v>
-      </c>
-      <c r="AG5" s="10">
-        <f t="shared" si="0"/>
-        <v>44714</v>
-      </c>
-      <c r="AH5" s="10">
-        <f t="shared" si="0"/>
-        <v>44715</v>
-      </c>
-      <c r="AI5" s="10">
-        <f t="shared" si="0"/>
-        <v>44716</v>
-      </c>
-      <c r="AJ5" s="12">
-        <f t="shared" si="0"/>
-        <v>44717</v>
-      </c>
-      <c r="AK5" s="11">
-        <f>AJ5+1</f>
-        <v>44718</v>
-      </c>
-      <c r="AL5" s="10">
-        <f>AK5+1</f>
-        <v>44719</v>
-      </c>
-      <c r="AM5" s="10">
-        <f t="shared" si="0"/>
-        <v>44720</v>
-      </c>
-      <c r="AN5" s="10">
-        <f t="shared" si="0"/>
-        <v>44721</v>
-      </c>
-      <c r="AO5" s="10">
-        <f t="shared" si="0"/>
-        <v>44722</v>
-      </c>
-      <c r="AP5" s="10">
-        <f t="shared" si="0"/>
-        <v>44723</v>
-      </c>
-      <c r="AQ5" s="12">
-        <f t="shared" si="0"/>
-        <v>44724</v>
-      </c>
-      <c r="AR5" s="11">
-        <f>AQ5+1</f>
-        <v>44725</v>
-      </c>
-      <c r="AS5" s="10">
-        <f>AR5+1</f>
-        <v>44726</v>
-      </c>
-      <c r="AT5" s="10">
-        <f t="shared" si="0"/>
-        <v>44727</v>
-      </c>
-      <c r="AU5" s="10">
-        <f t="shared" si="0"/>
-        <v>44728</v>
-      </c>
-      <c r="AV5" s="10">
-        <f t="shared" si="0"/>
-        <v>44729</v>
-      </c>
-      <c r="AW5" s="10">
-        <f t="shared" si="0"/>
-        <v>44730</v>
-      </c>
-      <c r="AX5" s="12">
-        <f t="shared" si="0"/>
-        <v>44731</v>
-      </c>
-      <c r="AY5" s="11">
-        <f>AX5+1</f>
-        <v>44732</v>
-      </c>
-      <c r="AZ5" s="10">
-        <f>AY5+1</f>
-        <v>44733</v>
-      </c>
-      <c r="BA5" s="10">
-        <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
-        <v>44734</v>
-      </c>
-      <c r="BB5" s="10">
-        <f t="shared" si="1"/>
-        <v>44735</v>
-      </c>
-      <c r="BC5" s="10">
-        <f t="shared" si="1"/>
-        <v>44736</v>
-      </c>
-      <c r="BD5" s="10">
-        <f t="shared" si="1"/>
-        <v>44737</v>
-      </c>
-      <c r="BE5" s="12">
-        <f t="shared" si="1"/>
-        <v>44738</v>
-      </c>
-      <c r="BF5" s="11">
-        <f>BE5+1</f>
-        <v>44739</v>
-      </c>
-      <c r="BG5" s="10">
-        <f>BF5+1</f>
-        <v>44740</v>
-      </c>
-      <c r="BH5" s="10">
-        <f t="shared" ref="BH5:BL5" si="2">BG5+1</f>
-        <v>44741</v>
-      </c>
-      <c r="BI5" s="10">
-        <f t="shared" si="2"/>
-        <v>44742</v>
-      </c>
-      <c r="BJ5" s="10">
-        <f t="shared" si="2"/>
-        <v>44743</v>
-      </c>
-      <c r="BK5" s="10">
-        <f t="shared" si="2"/>
-        <v>44744</v>
-      </c>
-      <c r="BL5" s="12">
-        <f t="shared" si="2"/>
-        <v>44745</v>
-      </c>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="59" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="I6" s="13" t="str">
-        <f t="shared" ref="I6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
+        <f t="shared" ref="I6" si="1">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
       </c>
       <c r="J6" s="13" t="str">
-        <f t="shared" ref="J6:AR6" si="4">LEFT(TEXT(J5,"ddd"),1)</f>
+        <f t="shared" ref="J6:AC6" si="2">LEFT(TEXT(J5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="K6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>W</v>
       </c>
       <c r="L6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>T</v>
       </c>
       <c r="M6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>F</v>
       </c>
       <c r="N6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="O6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="P6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>M</v>
       </c>
       <c r="Q6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>T</v>
       </c>
       <c r="R6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>W</v>
       </c>
       <c r="S6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>T</v>
       </c>
       <c r="T6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>F</v>
       </c>
       <c r="U6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="V6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="W6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>M</v>
       </c>
       <c r="X6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>T</v>
       </c>
       <c r="Y6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>W</v>
       </c>
       <c r="Z6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>T</v>
       </c>
       <c r="AA6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>F</v>
       </c>
       <c r="AB6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
       <c r="AC6" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>S</v>
-      </c>
-      <c r="AD6" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>M</v>
-      </c>
-      <c r="AE6" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>T</v>
-      </c>
-      <c r="AF6" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>W</v>
-      </c>
-      <c r="AG6" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>T</v>
-      </c>
-      <c r="AH6" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>F</v>
-      </c>
-      <c r="AI6" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>S</v>
-      </c>
-      <c r="AJ6" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>S</v>
-      </c>
-      <c r="AK6" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>M</v>
-      </c>
-      <c r="AL6" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>T</v>
-      </c>
-      <c r="AM6" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>W</v>
-      </c>
-      <c r="AN6" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>T</v>
-      </c>
-      <c r="AO6" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>F</v>
-      </c>
-      <c r="AP6" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>S</v>
-      </c>
-      <c r="AQ6" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>S</v>
-      </c>
-      <c r="AR6" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v>M</v>
-      </c>
-      <c r="AS6" s="13" t="str">
-        <f t="shared" ref="AS6:BL6" si="5">LEFT(TEXT(AS5,"ddd"),1)</f>
-        <v>T</v>
-      </c>
-      <c r="AT6" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>W</v>
-      </c>
-      <c r="AU6" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>T</v>
-      </c>
-      <c r="AV6" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>F</v>
-      </c>
-      <c r="AW6" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>S</v>
-      </c>
-      <c r="AX6" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>S</v>
-      </c>
-      <c r="AY6" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>M</v>
-      </c>
-      <c r="AZ6" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>T</v>
-      </c>
-      <c r="BA6" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>W</v>
-      </c>
-      <c r="BB6" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>T</v>
-      </c>
-      <c r="BC6" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>F</v>
-      </c>
-      <c r="BD6" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>S</v>
-      </c>
-      <c r="BE6" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>S</v>
-      </c>
-      <c r="BF6" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>M</v>
-      </c>
-      <c r="BG6" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>T</v>
-      </c>
-      <c r="BH6" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>W</v>
-      </c>
-      <c r="BI6" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>T</v>
-      </c>
-      <c r="BJ6" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>F</v>
-      </c>
-      <c r="BK6" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>S</v>
-      </c>
-      <c r="BL6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>S</v>
       </c>
     </row>
     <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="58" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C7" s="61"/>
       <c r="E7"/>
@@ -2193,48 +1926,13 @@
       <c r="AA7" s="44"/>
       <c r="AB7" s="44"/>
       <c r="AC7" s="44"/>
-      <c r="AD7" s="44"/>
-      <c r="AE7" s="44"/>
-      <c r="AF7" s="44"/>
-      <c r="AG7" s="44"/>
-      <c r="AH7" s="44"/>
-      <c r="AI7" s="44"/>
-      <c r="AJ7" s="44"/>
-      <c r="AK7" s="44"/>
-      <c r="AL7" s="44"/>
-      <c r="AM7" s="44"/>
-      <c r="AN7" s="44"/>
-      <c r="AO7" s="44"/>
-      <c r="AP7" s="44"/>
-      <c r="AQ7" s="44"/>
-      <c r="AR7" s="44"/>
-      <c r="AS7" s="44"/>
-      <c r="AT7" s="44"/>
-      <c r="AU7" s="44"/>
-      <c r="AV7" s="44"/>
-      <c r="AW7" s="44"/>
-      <c r="AX7" s="44"/>
-      <c r="AY7" s="44"/>
-      <c r="AZ7" s="44"/>
-      <c r="BA7" s="44"/>
-      <c r="BB7" s="44"/>
-      <c r="BC7" s="44"/>
-      <c r="BD7" s="44"/>
-      <c r="BE7" s="44"/>
-      <c r="BF7" s="44"/>
-      <c r="BG7" s="44"/>
-      <c r="BH7" s="44"/>
-      <c r="BI7" s="44"/>
-      <c r="BJ7" s="44"/>
-      <c r="BK7" s="44"/>
-      <c r="BL7" s="44"/>
     </row>
     <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="59" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>40</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>47</v>
       </c>
       <c r="C8" s="66"/>
       <c r="D8" s="19"/>
@@ -2242,7 +1940,7 @@
       <c r="F8" s="21"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17" t="str">
-        <f t="shared" ref="H8:H34" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H40" si="3">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="44"/>
@@ -2266,51 +1964,51 @@
       <c r="AA8" s="44"/>
       <c r="AB8" s="44"/>
       <c r="AC8" s="44"/>
-      <c r="AD8" s="44"/>
-      <c r="AE8" s="44"/>
-      <c r="AF8" s="44"/>
-      <c r="AG8" s="44"/>
-      <c r="AH8" s="44"/>
-      <c r="AI8" s="44"/>
-      <c r="AJ8" s="44"/>
-      <c r="AK8" s="44"/>
-      <c r="AL8" s="44"/>
-      <c r="AM8" s="44"/>
-      <c r="AN8" s="44"/>
-      <c r="AO8" s="44"/>
-      <c r="AP8" s="44"/>
-      <c r="AQ8" s="44"/>
-      <c r="AR8" s="44"/>
-      <c r="AS8" s="44"/>
-      <c r="AT8" s="44"/>
-      <c r="AU8" s="44"/>
-      <c r="AV8" s="44"/>
-      <c r="AW8" s="44"/>
-      <c r="AX8" s="44"/>
-      <c r="AY8" s="44"/>
-      <c r="AZ8" s="44"/>
-      <c r="BA8" s="44"/>
-      <c r="BB8" s="44"/>
-      <c r="BC8" s="44"/>
-      <c r="BD8" s="44"/>
-      <c r="BE8" s="44"/>
-      <c r="BF8" s="44"/>
-      <c r="BG8" s="44"/>
-      <c r="BH8" s="44"/>
-      <c r="BI8" s="44"/>
-      <c r="BJ8" s="44"/>
-      <c r="BK8" s="44"/>
-      <c r="BL8" s="44"/>
+      <c r="AD8"/>
+      <c r="AE8"/>
+      <c r="AF8"/>
+      <c r="AG8"/>
+      <c r="AH8"/>
+      <c r="AI8"/>
+      <c r="AJ8"/>
+      <c r="AK8"/>
+      <c r="AL8"/>
+      <c r="AM8"/>
+      <c r="AN8"/>
+      <c r="AO8"/>
+      <c r="AP8"/>
+      <c r="AQ8"/>
+      <c r="AR8"/>
+      <c r="AS8"/>
+      <c r="AT8"/>
+      <c r="AU8"/>
+      <c r="AV8"/>
+      <c r="AW8"/>
+      <c r="AX8"/>
+      <c r="AY8"/>
+      <c r="AZ8"/>
+      <c r="BA8"/>
+      <c r="BB8"/>
+      <c r="BC8"/>
+      <c r="BD8"/>
+      <c r="BE8"/>
+      <c r="BF8"/>
+      <c r="BG8"/>
+      <c r="BH8"/>
+      <c r="BI8"/>
+      <c r="BJ8"/>
+      <c r="BK8"/>
+      <c r="BL8"/>
     </row>
     <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="94" t="s">
-        <v>49</v>
+        <v>34</v>
+      </c>
+      <c r="B9" s="75" t="s">
+        <v>43</v>
       </c>
       <c r="C9" s="67" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="84">
@@ -2323,7 +2021,7 @@
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I9" s="44"/>
@@ -2347,51 +2045,51 @@
       <c r="AA9" s="44"/>
       <c r="AB9" s="44"/>
       <c r="AC9" s="44"/>
-      <c r="AD9" s="44"/>
-      <c r="AE9" s="44"/>
-      <c r="AF9" s="44"/>
-      <c r="AG9" s="44"/>
-      <c r="AH9" s="44"/>
-      <c r="AI9" s="44"/>
-      <c r="AJ9" s="44"/>
-      <c r="AK9" s="44"/>
-      <c r="AL9" s="44"/>
-      <c r="AM9" s="44"/>
-      <c r="AN9" s="44"/>
-      <c r="AO9" s="44"/>
-      <c r="AP9" s="44"/>
-      <c r="AQ9" s="44"/>
-      <c r="AR9" s="44"/>
-      <c r="AS9" s="44"/>
-      <c r="AT9" s="44"/>
-      <c r="AU9" s="44"/>
-      <c r="AV9" s="44"/>
-      <c r="AW9" s="44"/>
-      <c r="AX9" s="44"/>
-      <c r="AY9" s="44"/>
-      <c r="AZ9" s="44"/>
-      <c r="BA9" s="44"/>
-      <c r="BB9" s="44"/>
-      <c r="BC9" s="44"/>
-      <c r="BD9" s="44"/>
-      <c r="BE9" s="44"/>
-      <c r="BF9" s="44"/>
-      <c r="BG9" s="44"/>
-      <c r="BH9" s="44"/>
-      <c r="BI9" s="44"/>
-      <c r="BJ9" s="44"/>
-      <c r="BK9" s="44"/>
-      <c r="BL9" s="44"/>
+      <c r="AD9"/>
+      <c r="AE9"/>
+      <c r="AF9"/>
+      <c r="AG9"/>
+      <c r="AH9"/>
+      <c r="AI9"/>
+      <c r="AJ9"/>
+      <c r="AK9"/>
+      <c r="AL9"/>
+      <c r="AM9"/>
+      <c r="AN9"/>
+      <c r="AO9"/>
+      <c r="AP9"/>
+      <c r="AQ9"/>
+      <c r="AR9"/>
+      <c r="AS9"/>
+      <c r="AT9"/>
+      <c r="AU9"/>
+      <c r="AV9"/>
+      <c r="AW9"/>
+      <c r="AX9"/>
+      <c r="AY9"/>
+      <c r="AZ9"/>
+      <c r="BA9"/>
+      <c r="BB9"/>
+      <c r="BC9"/>
+      <c r="BD9"/>
+      <c r="BE9"/>
+      <c r="BF9"/>
+      <c r="BG9"/>
+      <c r="BH9"/>
+      <c r="BI9"/>
+      <c r="BJ9"/>
+      <c r="BK9"/>
+      <c r="BL9"/>
     </row>
     <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="59" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B10" s="75" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C10" s="67" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="84">
@@ -2404,7 +2102,7 @@
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="I10" s="44"/>
@@ -2428,49 +2126,49 @@
       <c r="AA10" s="44"/>
       <c r="AB10" s="44"/>
       <c r="AC10" s="44"/>
-      <c r="AD10" s="44"/>
-      <c r="AE10" s="44"/>
-      <c r="AF10" s="44"/>
-      <c r="AG10" s="44"/>
-      <c r="AH10" s="44"/>
-      <c r="AI10" s="44"/>
-      <c r="AJ10" s="44"/>
-      <c r="AK10" s="44"/>
-      <c r="AL10" s="44"/>
-      <c r="AM10" s="44"/>
-      <c r="AN10" s="44"/>
-      <c r="AO10" s="44"/>
-      <c r="AP10" s="44"/>
-      <c r="AQ10" s="44"/>
-      <c r="AR10" s="44"/>
-      <c r="AS10" s="44"/>
-      <c r="AT10" s="44"/>
-      <c r="AU10" s="44"/>
-      <c r="AV10" s="44"/>
-      <c r="AW10" s="44"/>
-      <c r="AX10" s="44"/>
-      <c r="AY10" s="44"/>
-      <c r="AZ10" s="44"/>
-      <c r="BA10" s="44"/>
-      <c r="BB10" s="44"/>
-      <c r="BC10" s="44"/>
-      <c r="BD10" s="44"/>
-      <c r="BE10" s="44"/>
-      <c r="BF10" s="44"/>
-      <c r="BG10" s="44"/>
-      <c r="BH10" s="44"/>
-      <c r="BI10" s="44"/>
-      <c r="BJ10" s="44"/>
-      <c r="BK10" s="44"/>
-      <c r="BL10" s="44"/>
+      <c r="AD10"/>
+      <c r="AE10"/>
+      <c r="AF10"/>
+      <c r="AG10"/>
+      <c r="AH10"/>
+      <c r="AI10"/>
+      <c r="AJ10"/>
+      <c r="AK10"/>
+      <c r="AL10"/>
+      <c r="AM10"/>
+      <c r="AN10"/>
+      <c r="AO10"/>
+      <c r="AP10"/>
+      <c r="AQ10"/>
+      <c r="AR10"/>
+      <c r="AS10"/>
+      <c r="AT10"/>
+      <c r="AU10"/>
+      <c r="AV10"/>
+      <c r="AW10"/>
+      <c r="AX10"/>
+      <c r="AY10"/>
+      <c r="AZ10"/>
+      <c r="BA10"/>
+      <c r="BB10"/>
+      <c r="BC10"/>
+      <c r="BD10"/>
+      <c r="BE10"/>
+      <c r="BF10"/>
+      <c r="BG10"/>
+      <c r="BH10"/>
+      <c r="BI10"/>
+      <c r="BJ10"/>
+      <c r="BK10"/>
+      <c r="BL10"/>
     </row>
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="58"/>
-      <c r="B11" s="75" t="s">
-        <v>51</v>
+      <c r="B11" s="88" t="s">
+        <v>42</v>
       </c>
       <c r="C11" s="67" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="84">
@@ -2483,7 +2181,7 @@
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I11" s="44"/>
@@ -2507,49 +2205,49 @@
       <c r="AA11" s="44"/>
       <c r="AB11" s="44"/>
       <c r="AC11" s="44"/>
-      <c r="AD11" s="44"/>
-      <c r="AE11" s="44"/>
-      <c r="AF11" s="44"/>
-      <c r="AG11" s="44"/>
-      <c r="AH11" s="44"/>
-      <c r="AI11" s="44"/>
-      <c r="AJ11" s="44"/>
-      <c r="AK11" s="44"/>
-      <c r="AL11" s="44"/>
-      <c r="AM11" s="44"/>
-      <c r="AN11" s="44"/>
-      <c r="AO11" s="44"/>
-      <c r="AP11" s="44"/>
-      <c r="AQ11" s="44"/>
-      <c r="AR11" s="44"/>
-      <c r="AS11" s="44"/>
-      <c r="AT11" s="44"/>
-      <c r="AU11" s="44"/>
-      <c r="AV11" s="44"/>
-      <c r="AW11" s="44"/>
-      <c r="AX11" s="44"/>
-      <c r="AY11" s="44"/>
-      <c r="AZ11" s="44"/>
-      <c r="BA11" s="44"/>
-      <c r="BB11" s="44"/>
-      <c r="BC11" s="44"/>
-      <c r="BD11" s="44"/>
-      <c r="BE11" s="44"/>
-      <c r="BF11" s="44"/>
-      <c r="BG11" s="44"/>
-      <c r="BH11" s="44"/>
-      <c r="BI11" s="44"/>
-      <c r="BJ11" s="44"/>
-      <c r="BK11" s="44"/>
-      <c r="BL11" s="44"/>
+      <c r="AD11"/>
+      <c r="AE11"/>
+      <c r="AF11"/>
+      <c r="AG11"/>
+      <c r="AH11"/>
+      <c r="AI11"/>
+      <c r="AJ11"/>
+      <c r="AK11"/>
+      <c r="AL11"/>
+      <c r="AM11"/>
+      <c r="AN11"/>
+      <c r="AO11"/>
+      <c r="AP11"/>
+      <c r="AQ11"/>
+      <c r="AR11"/>
+      <c r="AS11"/>
+      <c r="AT11"/>
+      <c r="AU11"/>
+      <c r="AV11"/>
+      <c r="AW11"/>
+      <c r="AX11"/>
+      <c r="AY11"/>
+      <c r="AZ11"/>
+      <c r="BA11"/>
+      <c r="BB11"/>
+      <c r="BC11"/>
+      <c r="BD11"/>
+      <c r="BE11"/>
+      <c r="BF11"/>
+      <c r="BG11"/>
+      <c r="BH11"/>
+      <c r="BI11"/>
+      <c r="BJ11"/>
+      <c r="BK11"/>
+      <c r="BL11"/>
     </row>
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="58"/>
       <c r="B12" s="75" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C12" s="67" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="84">
@@ -2557,13 +2255,13 @@
         <v>44692</v>
       </c>
       <c r="F12" s="84">
-        <f>E12+1</f>
-        <v>44693</v>
+        <f>E12</f>
+        <v>44692</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="17">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="I12" s="44"/>
       <c r="J12" s="44"/>
@@ -2586,53 +2284,53 @@
       <c r="AA12" s="44"/>
       <c r="AB12" s="44"/>
       <c r="AC12" s="44"/>
-      <c r="AD12" s="44"/>
-      <c r="AE12" s="44"/>
-      <c r="AF12" s="44"/>
-      <c r="AG12" s="44"/>
-      <c r="AH12" s="44"/>
-      <c r="AI12" s="44"/>
-      <c r="AJ12" s="44"/>
-      <c r="AK12" s="44"/>
-      <c r="AL12" s="44"/>
-      <c r="AM12" s="44"/>
-      <c r="AN12" s="44"/>
-      <c r="AO12" s="44"/>
-      <c r="AP12" s="44"/>
-      <c r="AQ12" s="44"/>
-      <c r="AR12" s="44"/>
-      <c r="AS12" s="44"/>
-      <c r="AT12" s="44"/>
-      <c r="AU12" s="44"/>
-      <c r="AV12" s="44"/>
-      <c r="AW12" s="44"/>
-      <c r="AX12" s="44"/>
-      <c r="AY12" s="44"/>
-      <c r="AZ12" s="44"/>
-      <c r="BA12" s="44"/>
-      <c r="BB12" s="44"/>
-      <c r="BC12" s="44"/>
-      <c r="BD12" s="44"/>
-      <c r="BE12" s="44"/>
-      <c r="BF12" s="44"/>
-      <c r="BG12" s="44"/>
-      <c r="BH12" s="44"/>
-      <c r="BI12" s="44"/>
-      <c r="BJ12" s="44"/>
-      <c r="BK12" s="44"/>
-      <c r="BL12" s="44"/>
+      <c r="AD12"/>
+      <c r="AE12"/>
+      <c r="AF12"/>
+      <c r="AG12"/>
+      <c r="AH12"/>
+      <c r="AI12"/>
+      <c r="AJ12"/>
+      <c r="AK12"/>
+      <c r="AL12"/>
+      <c r="AM12"/>
+      <c r="AN12"/>
+      <c r="AO12"/>
+      <c r="AP12"/>
+      <c r="AQ12"/>
+      <c r="AR12"/>
+      <c r="AS12"/>
+      <c r="AT12"/>
+      <c r="AU12"/>
+      <c r="AV12"/>
+      <c r="AW12"/>
+      <c r="AX12"/>
+      <c r="AY12"/>
+      <c r="AZ12"/>
+      <c r="BA12"/>
+      <c r="BB12"/>
+      <c r="BC12"/>
+      <c r="BD12"/>
+      <c r="BE12"/>
+      <c r="BF12"/>
+      <c r="BG12"/>
+      <c r="BH12"/>
+      <c r="BI12"/>
+      <c r="BJ12"/>
+      <c r="BK12"/>
+      <c r="BL12"/>
     </row>
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="58"/>
       <c r="B13" s="75" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C13" s="67" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="84">
-        <f>E10+1</f>
+        <f>E12</f>
         <v>44692</v>
       </c>
       <c r="F13" s="84">
@@ -2640,10 +2338,7 @@
         <v>44693</v>
       </c>
       <c r="G13" s="17"/>
-      <c r="H13" s="17">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
+      <c r="H13" s="17"/>
       <c r="I13" s="44"/>
       <c r="J13" s="44"/>
       <c r="K13" s="44"/>
@@ -2660,62 +2355,68 @@
       <c r="V13" s="44"/>
       <c r="W13" s="44"/>
       <c r="X13" s="44"/>
-      <c r="Y13" s="44"/>
+      <c r="Y13" s="45"/>
       <c r="Z13" s="44"/>
       <c r="AA13" s="44"/>
       <c r="AB13" s="44"/>
       <c r="AC13" s="44"/>
-      <c r="AD13" s="44"/>
-      <c r="AE13" s="44"/>
-      <c r="AF13" s="44"/>
-      <c r="AG13" s="44"/>
-      <c r="AH13" s="44"/>
-      <c r="AI13" s="44"/>
-      <c r="AJ13" s="44"/>
-      <c r="AK13" s="44"/>
-      <c r="AL13" s="44"/>
-      <c r="AM13" s="44"/>
-      <c r="AN13" s="44"/>
-      <c r="AO13" s="44"/>
-      <c r="AP13" s="44"/>
-      <c r="AQ13" s="44"/>
-      <c r="AR13" s="44"/>
-      <c r="AS13" s="44"/>
-      <c r="AT13" s="44"/>
-      <c r="AU13" s="44"/>
-      <c r="AV13" s="44"/>
-      <c r="AW13" s="44"/>
-      <c r="AX13" s="44"/>
-      <c r="AY13" s="44"/>
-      <c r="AZ13" s="44"/>
-      <c r="BA13" s="44"/>
-      <c r="BB13" s="44"/>
-      <c r="BC13" s="44"/>
-      <c r="BD13" s="44"/>
-      <c r="BE13" s="44"/>
-      <c r="BF13" s="44"/>
-      <c r="BG13" s="44"/>
-      <c r="BH13" s="44"/>
-      <c r="BI13" s="44"/>
-      <c r="BJ13" s="44"/>
-      <c r="BK13" s="44"/>
-      <c r="BL13" s="44"/>
+      <c r="AD13"/>
+      <c r="AE13"/>
+      <c r="AF13"/>
+      <c r="AG13"/>
+      <c r="AH13"/>
+      <c r="AI13"/>
+      <c r="AJ13"/>
+      <c r="AK13"/>
+      <c r="AL13"/>
+      <c r="AM13"/>
+      <c r="AN13"/>
+      <c r="AO13"/>
+      <c r="AP13"/>
+      <c r="AQ13"/>
+      <c r="AR13"/>
+      <c r="AS13"/>
+      <c r="AT13"/>
+      <c r="AU13"/>
+      <c r="AV13"/>
+      <c r="AW13"/>
+      <c r="AX13"/>
+      <c r="AY13"/>
+      <c r="AZ13"/>
+      <c r="BA13"/>
+      <c r="BB13"/>
+      <c r="BC13"/>
+      <c r="BD13"/>
+      <c r="BE13"/>
+      <c r="BF13"/>
+      <c r="BG13"/>
+      <c r="BH13"/>
+      <c r="BI13"/>
+      <c r="BJ13"/>
+      <c r="BK13"/>
+      <c r="BL13"/>
     </row>
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="59" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="68"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="26"/>
+      <c r="A14" s="58"/>
+      <c r="B14" s="75" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="84">
+        <f>F13</f>
+        <v>44693</v>
+      </c>
+      <c r="F14" s="84">
+        <f>E14</f>
+        <v>44693</v>
+      </c>
       <c r="G14" s="17"/>
-      <c r="H14" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
+      <c r="H14" s="17">
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="I14" s="44"/>
       <c r="J14" s="44"/>
@@ -2738,63 +2439,57 @@
       <c r="AA14" s="44"/>
       <c r="AB14" s="44"/>
       <c r="AC14" s="44"/>
-      <c r="AD14" s="44"/>
-      <c r="AE14" s="44"/>
-      <c r="AF14" s="44"/>
-      <c r="AG14" s="44"/>
-      <c r="AH14" s="44"/>
-      <c r="AI14" s="44"/>
-      <c r="AJ14" s="44"/>
-      <c r="AK14" s="44"/>
-      <c r="AL14" s="44"/>
-      <c r="AM14" s="44"/>
-      <c r="AN14" s="44"/>
-      <c r="AO14" s="44"/>
-      <c r="AP14" s="44"/>
-      <c r="AQ14" s="44"/>
-      <c r="AR14" s="44"/>
-      <c r="AS14" s="44"/>
-      <c r="AT14" s="44"/>
-      <c r="AU14" s="44"/>
-      <c r="AV14" s="44"/>
-      <c r="AW14" s="44"/>
-      <c r="AX14" s="44"/>
-      <c r="AY14" s="44"/>
-      <c r="AZ14" s="44"/>
-      <c r="BA14" s="44"/>
-      <c r="BB14" s="44"/>
-      <c r="BC14" s="44"/>
-      <c r="BD14" s="44"/>
-      <c r="BE14" s="44"/>
-      <c r="BF14" s="44"/>
-      <c r="BG14" s="44"/>
-      <c r="BH14" s="44"/>
-      <c r="BI14" s="44"/>
-      <c r="BJ14" s="44"/>
-      <c r="BK14" s="44"/>
-      <c r="BL14" s="44"/>
+      <c r="AD14"/>
+      <c r="AE14"/>
+      <c r="AF14"/>
+      <c r="AG14"/>
+      <c r="AH14"/>
+      <c r="AI14"/>
+      <c r="AJ14"/>
+      <c r="AK14"/>
+      <c r="AL14"/>
+      <c r="AM14"/>
+      <c r="AN14"/>
+      <c r="AO14"/>
+      <c r="AP14"/>
+      <c r="AQ14"/>
+      <c r="AR14"/>
+      <c r="AS14"/>
+      <c r="AT14"/>
+      <c r="AU14"/>
+      <c r="AV14"/>
+      <c r="AW14"/>
+      <c r="AX14"/>
+      <c r="AY14"/>
+      <c r="AZ14"/>
+      <c r="BA14"/>
+      <c r="BB14"/>
+      <c r="BC14"/>
+      <c r="BD14"/>
+      <c r="BE14"/>
+      <c r="BF14"/>
+      <c r="BG14"/>
+      <c r="BH14"/>
+      <c r="BI14"/>
+      <c r="BJ14"/>
+      <c r="BK14"/>
+      <c r="BL14"/>
     </row>
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="59"/>
-      <c r="B15" s="76" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="69" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="85">
-        <f>F13+1</f>
-        <v>44694</v>
-      </c>
-      <c r="F15" s="85">
-        <f>E15</f>
-        <v>44694</v>
-      </c>
+      <c r="A15" s="59" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="68"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="26"/>
       <c r="G15" s="17"/>
-      <c r="H15" s="17">
-        <f t="shared" si="6"/>
-        <v>1</v>
+      <c r="H15" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="I15" s="44"/>
       <c r="J15" s="44"/>
@@ -2817,53 +2512,53 @@
       <c r="AA15" s="44"/>
       <c r="AB15" s="44"/>
       <c r="AC15" s="44"/>
-      <c r="AD15" s="44"/>
-      <c r="AE15" s="44"/>
-      <c r="AF15" s="44"/>
-      <c r="AG15" s="44"/>
-      <c r="AH15" s="44"/>
-      <c r="AI15" s="44"/>
-      <c r="AJ15" s="44"/>
-      <c r="AK15" s="44"/>
-      <c r="AL15" s="44"/>
-      <c r="AM15" s="44"/>
-      <c r="AN15" s="44"/>
-      <c r="AO15" s="44"/>
-      <c r="AP15" s="44"/>
-      <c r="AQ15" s="44"/>
-      <c r="AR15" s="44"/>
-      <c r="AS15" s="44"/>
-      <c r="AT15" s="44"/>
-      <c r="AU15" s="44"/>
-      <c r="AV15" s="44"/>
-      <c r="AW15" s="44"/>
-      <c r="AX15" s="44"/>
-      <c r="AY15" s="44"/>
-      <c r="AZ15" s="44"/>
-      <c r="BA15" s="44"/>
-      <c r="BB15" s="44"/>
-      <c r="BC15" s="44"/>
-      <c r="BD15" s="44"/>
-      <c r="BE15" s="44"/>
-      <c r="BF15" s="44"/>
-      <c r="BG15" s="44"/>
-      <c r="BH15" s="44"/>
-      <c r="BI15" s="44"/>
-      <c r="BJ15" s="44"/>
-      <c r="BK15" s="44"/>
-      <c r="BL15" s="44"/>
+      <c r="AD15"/>
+      <c r="AE15"/>
+      <c r="AF15"/>
+      <c r="AG15"/>
+      <c r="AH15"/>
+      <c r="AI15"/>
+      <c r="AJ15"/>
+      <c r="AK15"/>
+      <c r="AL15"/>
+      <c r="AM15"/>
+      <c r="AN15"/>
+      <c r="AO15"/>
+      <c r="AP15"/>
+      <c r="AQ15"/>
+      <c r="AR15"/>
+      <c r="AS15"/>
+      <c r="AT15"/>
+      <c r="AU15"/>
+      <c r="AV15"/>
+      <c r="AW15"/>
+      <c r="AX15"/>
+      <c r="AY15"/>
+      <c r="AZ15"/>
+      <c r="BA15"/>
+      <c r="BB15"/>
+      <c r="BC15"/>
+      <c r="BD15"/>
+      <c r="BE15"/>
+      <c r="BF15"/>
+      <c r="BG15"/>
+      <c r="BH15"/>
+      <c r="BI15"/>
+      <c r="BJ15"/>
+      <c r="BK15"/>
+      <c r="BL15"/>
     </row>
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="58"/>
+      <c r="A16" s="59"/>
       <c r="B16" s="76" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C16" s="69" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D16" s="27"/>
       <c r="E16" s="85">
-        <f>E15</f>
+        <f>F14+1</f>
         <v>44694</v>
       </c>
       <c r="F16" s="85">
@@ -2872,7 +2567,7 @@
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I16" s="44"/>
@@ -2887,8 +2582,8 @@
       <c r="R16" s="44"/>
       <c r="S16" s="44"/>
       <c r="T16" s="44"/>
-      <c r="U16" s="45"/>
-      <c r="V16" s="45"/>
+      <c r="U16" s="44"/>
+      <c r="V16" s="44"/>
       <c r="W16" s="44"/>
       <c r="X16" s="44"/>
       <c r="Y16" s="44"/>
@@ -2896,63 +2591,63 @@
       <c r="AA16" s="44"/>
       <c r="AB16" s="44"/>
       <c r="AC16" s="44"/>
-      <c r="AD16" s="44"/>
-      <c r="AE16" s="44"/>
-      <c r="AF16" s="44"/>
-      <c r="AG16" s="44"/>
-      <c r="AH16" s="44"/>
-      <c r="AI16" s="44"/>
-      <c r="AJ16" s="44"/>
-      <c r="AK16" s="44"/>
-      <c r="AL16" s="44"/>
-      <c r="AM16" s="44"/>
-      <c r="AN16" s="44"/>
-      <c r="AO16" s="44"/>
-      <c r="AP16" s="44"/>
-      <c r="AQ16" s="44"/>
-      <c r="AR16" s="44"/>
-      <c r="AS16" s="44"/>
-      <c r="AT16" s="44"/>
-      <c r="AU16" s="44"/>
-      <c r="AV16" s="44"/>
-      <c r="AW16" s="44"/>
-      <c r="AX16" s="44"/>
-      <c r="AY16" s="44"/>
-      <c r="AZ16" s="44"/>
-      <c r="BA16" s="44"/>
-      <c r="BB16" s="44"/>
-      <c r="BC16" s="44"/>
-      <c r="BD16" s="44"/>
-      <c r="BE16" s="44"/>
-      <c r="BF16" s="44"/>
-      <c r="BG16" s="44"/>
-      <c r="BH16" s="44"/>
-      <c r="BI16" s="44"/>
-      <c r="BJ16" s="44"/>
-      <c r="BK16" s="44"/>
-      <c r="BL16" s="44"/>
+      <c r="AD16"/>
+      <c r="AE16"/>
+      <c r="AF16"/>
+      <c r="AG16"/>
+      <c r="AH16"/>
+      <c r="AI16"/>
+      <c r="AJ16"/>
+      <c r="AK16"/>
+      <c r="AL16"/>
+      <c r="AM16"/>
+      <c r="AN16"/>
+      <c r="AO16"/>
+      <c r="AP16"/>
+      <c r="AQ16"/>
+      <c r="AR16"/>
+      <c r="AS16"/>
+      <c r="AT16"/>
+      <c r="AU16"/>
+      <c r="AV16"/>
+      <c r="AW16"/>
+      <c r="AX16"/>
+      <c r="AY16"/>
+      <c r="AZ16"/>
+      <c r="BA16"/>
+      <c r="BB16"/>
+      <c r="BC16"/>
+      <c r="BD16"/>
+      <c r="BE16"/>
+      <c r="BF16"/>
+      <c r="BG16"/>
+      <c r="BH16"/>
+      <c r="BI16"/>
+      <c r="BJ16"/>
+      <c r="BK16"/>
+      <c r="BL16"/>
     </row>
     <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="58"/>
       <c r="B17" s="76" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C17" s="69" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D17" s="27"/>
       <c r="E17" s="85">
-        <f>F16</f>
+        <f>E16</f>
         <v>44694</v>
       </c>
       <c r="F17" s="85">
-        <f>E17+1</f>
-        <v>44695</v>
+        <f>E17</f>
+        <v>44694</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="I17" s="44"/>
       <c r="J17" s="44"/>
@@ -2966,8 +2661,8 @@
       <c r="R17" s="44"/>
       <c r="S17" s="44"/>
       <c r="T17" s="44"/>
-      <c r="U17" s="44"/>
-      <c r="V17" s="44"/>
+      <c r="U17" s="45"/>
+      <c r="V17" s="45"/>
       <c r="W17" s="44"/>
       <c r="X17" s="44"/>
       <c r="Y17" s="44"/>
@@ -2975,61 +2670,64 @@
       <c r="AA17" s="44"/>
       <c r="AB17" s="44"/>
       <c r="AC17" s="44"/>
-      <c r="AD17" s="44"/>
-      <c r="AE17" s="44"/>
-      <c r="AF17" s="44"/>
-      <c r="AG17" s="44"/>
-      <c r="AH17" s="44"/>
-      <c r="AI17" s="44"/>
-      <c r="AJ17" s="44"/>
-      <c r="AK17" s="44"/>
-      <c r="AL17" s="44"/>
-      <c r="AM17" s="44"/>
-      <c r="AN17" s="44"/>
-      <c r="AO17" s="44"/>
-      <c r="AP17" s="44"/>
-      <c r="AQ17" s="44"/>
-      <c r="AR17" s="44"/>
-      <c r="AS17" s="44"/>
-      <c r="AT17" s="44"/>
-      <c r="AU17" s="44"/>
-      <c r="AV17" s="44"/>
-      <c r="AW17" s="44"/>
-      <c r="AX17" s="44"/>
-      <c r="AY17" s="44"/>
-      <c r="AZ17" s="44"/>
-      <c r="BA17" s="44"/>
-      <c r="BB17" s="44"/>
-      <c r="BC17" s="44"/>
-      <c r="BD17" s="44"/>
-      <c r="BE17" s="44"/>
-      <c r="BF17" s="44"/>
-      <c r="BG17" s="44"/>
-      <c r="BH17" s="44"/>
-      <c r="BI17" s="44"/>
-      <c r="BJ17" s="44"/>
-      <c r="BK17" s="44"/>
-      <c r="BL17" s="44"/>
+      <c r="AD17"/>
+      <c r="AE17"/>
+      <c r="AF17"/>
+      <c r="AG17"/>
+      <c r="AH17"/>
+      <c r="AI17"/>
+      <c r="AJ17"/>
+      <c r="AK17"/>
+      <c r="AL17"/>
+      <c r="AM17"/>
+      <c r="AN17"/>
+      <c r="AO17"/>
+      <c r="AP17"/>
+      <c r="AQ17"/>
+      <c r="AR17"/>
+      <c r="AS17"/>
+      <c r="AT17"/>
+      <c r="AU17"/>
+      <c r="AV17"/>
+      <c r="AW17"/>
+      <c r="AX17"/>
+      <c r="AY17"/>
+      <c r="AZ17"/>
+      <c r="BA17"/>
+      <c r="BB17"/>
+      <c r="BC17"/>
+      <c r="BD17"/>
+      <c r="BE17"/>
+      <c r="BF17"/>
+      <c r="BG17"/>
+      <c r="BH17"/>
+      <c r="BI17"/>
+      <c r="BJ17"/>
+      <c r="BK17"/>
+      <c r="BL17"/>
     </row>
     <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="58"/>
       <c r="B18" s="76" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C18" s="69" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D18" s="27"/>
       <c r="E18" s="85">
         <f>F17</f>
+        <v>44694</v>
+      </c>
+      <c r="F18" s="85">
+        <f>E18+1</f>
         <v>44695</v>
       </c>
-      <c r="F18" s="85">
-        <f>E18</f>
-        <v>44695</v>
-      </c>
       <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
+      <c r="H18" s="17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
       <c r="I18" s="44"/>
       <c r="J18" s="44"/>
       <c r="K18" s="44"/>
@@ -3051,53 +2749,53 @@
       <c r="AA18" s="44"/>
       <c r="AB18" s="44"/>
       <c r="AC18" s="44"/>
-      <c r="AD18" s="44"/>
-      <c r="AE18" s="44"/>
-      <c r="AF18" s="44"/>
-      <c r="AG18" s="44"/>
-      <c r="AH18" s="44"/>
-      <c r="AI18" s="44"/>
-      <c r="AJ18" s="44"/>
-      <c r="AK18" s="44"/>
-      <c r="AL18" s="44"/>
-      <c r="AM18" s="44"/>
-      <c r="AN18" s="44"/>
-      <c r="AO18" s="44"/>
-      <c r="AP18" s="44"/>
-      <c r="AQ18" s="44"/>
-      <c r="AR18" s="44"/>
-      <c r="AS18" s="44"/>
-      <c r="AT18" s="44"/>
-      <c r="AU18" s="44"/>
-      <c r="AV18" s="44"/>
-      <c r="AW18" s="44"/>
-      <c r="AX18" s="44"/>
-      <c r="AY18" s="44"/>
-      <c r="AZ18" s="44"/>
-      <c r="BA18" s="44"/>
-      <c r="BB18" s="44"/>
-      <c r="BC18" s="44"/>
-      <c r="BD18" s="44"/>
-      <c r="BE18" s="44"/>
-      <c r="BF18" s="44"/>
-      <c r="BG18" s="44"/>
-      <c r="BH18" s="44"/>
-      <c r="BI18" s="44"/>
-      <c r="BJ18" s="44"/>
-      <c r="BK18" s="44"/>
-      <c r="BL18" s="44"/>
+      <c r="AD18"/>
+      <c r="AE18"/>
+      <c r="AF18"/>
+      <c r="AG18"/>
+      <c r="AH18"/>
+      <c r="AI18"/>
+      <c r="AJ18"/>
+      <c r="AK18"/>
+      <c r="AL18"/>
+      <c r="AM18"/>
+      <c r="AN18"/>
+      <c r="AO18"/>
+      <c r="AP18"/>
+      <c r="AQ18"/>
+      <c r="AR18"/>
+      <c r="AS18"/>
+      <c r="AT18"/>
+      <c r="AU18"/>
+      <c r="AV18"/>
+      <c r="AW18"/>
+      <c r="AX18"/>
+      <c r="AY18"/>
+      <c r="AZ18"/>
+      <c r="BA18"/>
+      <c r="BB18"/>
+      <c r="BC18"/>
+      <c r="BD18"/>
+      <c r="BE18"/>
+      <c r="BF18"/>
+      <c r="BG18"/>
+      <c r="BH18"/>
+      <c r="BI18"/>
+      <c r="BJ18"/>
+      <c r="BK18"/>
+      <c r="BL18"/>
     </row>
     <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="58"/>
       <c r="B19" s="76" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C19" s="69" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D19" s="27"/>
       <c r="E19" s="85">
-        <f>E18</f>
+        <f>F18</f>
         <v>44695</v>
       </c>
       <c r="F19" s="85">
@@ -3105,10 +2803,7 @@
         <v>44695</v>
       </c>
       <c r="G19" s="17"/>
-      <c r="H19" s="17">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
+      <c r="H19" s="17"/>
       <c r="I19" s="44"/>
       <c r="J19" s="44"/>
       <c r="K19" s="44"/>
@@ -3125,67 +2820,67 @@
       <c r="V19" s="44"/>
       <c r="W19" s="44"/>
       <c r="X19" s="44"/>
-      <c r="Y19" s="45"/>
+      <c r="Y19" s="44"/>
       <c r="Z19" s="44"/>
       <c r="AA19" s="44"/>
       <c r="AB19" s="44"/>
       <c r="AC19" s="44"/>
-      <c r="AD19" s="44"/>
-      <c r="AE19" s="44"/>
-      <c r="AF19" s="44"/>
-      <c r="AG19" s="44"/>
-      <c r="AH19" s="44"/>
-      <c r="AI19" s="44"/>
-      <c r="AJ19" s="44"/>
-      <c r="AK19" s="44"/>
-      <c r="AL19" s="44"/>
-      <c r="AM19" s="44"/>
-      <c r="AN19" s="44"/>
-      <c r="AO19" s="44"/>
-      <c r="AP19" s="44"/>
-      <c r="AQ19" s="44"/>
-      <c r="AR19" s="44"/>
-      <c r="AS19" s="44"/>
-      <c r="AT19" s="44"/>
-      <c r="AU19" s="44"/>
-      <c r="AV19" s="44"/>
-      <c r="AW19" s="44"/>
-      <c r="AX19" s="44"/>
-      <c r="AY19" s="44"/>
-      <c r="AZ19" s="44"/>
-      <c r="BA19" s="44"/>
-      <c r="BB19" s="44"/>
-      <c r="BC19" s="44"/>
-      <c r="BD19" s="44"/>
-      <c r="BE19" s="44"/>
-      <c r="BF19" s="44"/>
-      <c r="BG19" s="44"/>
-      <c r="BH19" s="44"/>
-      <c r="BI19" s="44"/>
-      <c r="BJ19" s="44"/>
-      <c r="BK19" s="44"/>
-      <c r="BL19" s="44"/>
+      <c r="AD19"/>
+      <c r="AE19"/>
+      <c r="AF19"/>
+      <c r="AG19"/>
+      <c r="AH19"/>
+      <c r="AI19"/>
+      <c r="AJ19"/>
+      <c r="AK19"/>
+      <c r="AL19"/>
+      <c r="AM19"/>
+      <c r="AN19"/>
+      <c r="AO19"/>
+      <c r="AP19"/>
+      <c r="AQ19"/>
+      <c r="AR19"/>
+      <c r="AS19"/>
+      <c r="AT19"/>
+      <c r="AU19"/>
+      <c r="AV19"/>
+      <c r="AW19"/>
+      <c r="AX19"/>
+      <c r="AY19"/>
+      <c r="AZ19"/>
+      <c r="BA19"/>
+      <c r="BB19"/>
+      <c r="BC19"/>
+      <c r="BD19"/>
+      <c r="BE19"/>
+      <c r="BF19"/>
+      <c r="BG19"/>
+      <c r="BH19"/>
+      <c r="BI19"/>
+      <c r="BJ19"/>
+      <c r="BK19"/>
+      <c r="BL19"/>
     </row>
     <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="58"/>
       <c r="B20" s="76" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C20" s="69" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D20" s="27"/>
       <c r="E20" s="85">
-        <f>E19+1</f>
-        <v>44696</v>
+        <f>E19</f>
+        <v>44695</v>
       </c>
       <c r="F20" s="85">
         <f>E20</f>
-        <v>44696</v>
+        <v>44695</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I20" s="44"/>
@@ -3204,62 +2899,68 @@
       <c r="V20" s="44"/>
       <c r="W20" s="44"/>
       <c r="X20" s="44"/>
-      <c r="Y20" s="44"/>
+      <c r="Y20" s="45"/>
       <c r="Z20" s="44"/>
       <c r="AA20" s="44"/>
       <c r="AB20" s="44"/>
       <c r="AC20" s="44"/>
-      <c r="AD20" s="44"/>
-      <c r="AE20" s="44"/>
-      <c r="AF20" s="44"/>
-      <c r="AG20" s="44"/>
-      <c r="AH20" s="44"/>
-      <c r="AI20" s="44"/>
-      <c r="AJ20" s="44"/>
-      <c r="AK20" s="44"/>
-      <c r="AL20" s="44"/>
-      <c r="AM20" s="44"/>
-      <c r="AN20" s="44"/>
-      <c r="AO20" s="44"/>
-      <c r="AP20" s="44"/>
-      <c r="AQ20" s="44"/>
-      <c r="AR20" s="44"/>
-      <c r="AS20" s="44"/>
-      <c r="AT20" s="44"/>
-      <c r="AU20" s="44"/>
-      <c r="AV20" s="44"/>
-      <c r="AW20" s="44"/>
-      <c r="AX20" s="44"/>
-      <c r="AY20" s="44"/>
-      <c r="AZ20" s="44"/>
-      <c r="BA20" s="44"/>
-      <c r="BB20" s="44"/>
-      <c r="BC20" s="44"/>
-      <c r="BD20" s="44"/>
-      <c r="BE20" s="44"/>
-      <c r="BF20" s="44"/>
-      <c r="BG20" s="44"/>
-      <c r="BH20" s="44"/>
-      <c r="BI20" s="44"/>
-      <c r="BJ20" s="44"/>
-      <c r="BK20" s="44"/>
-      <c r="BL20" s="44"/>
+      <c r="AD20"/>
+      <c r="AE20"/>
+      <c r="AF20"/>
+      <c r="AG20"/>
+      <c r="AH20"/>
+      <c r="AI20"/>
+      <c r="AJ20"/>
+      <c r="AK20"/>
+      <c r="AL20"/>
+      <c r="AM20"/>
+      <c r="AN20"/>
+      <c r="AO20"/>
+      <c r="AP20"/>
+      <c r="AQ20"/>
+      <c r="AR20"/>
+      <c r="AS20"/>
+      <c r="AT20"/>
+      <c r="AU20"/>
+      <c r="AV20"/>
+      <c r="AW20"/>
+      <c r="AX20"/>
+      <c r="AY20"/>
+      <c r="AZ20"/>
+      <c r="BA20"/>
+      <c r="BB20"/>
+      <c r="BC20"/>
+      <c r="BD20"/>
+      <c r="BE20"/>
+      <c r="BF20"/>
+      <c r="BG20"/>
+      <c r="BH20"/>
+      <c r="BI20"/>
+      <c r="BJ20"/>
+      <c r="BK20"/>
+      <c r="BL20"/>
     </row>
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="70"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="31"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="76" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="69" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="27"/>
+      <c r="E21" s="85">
+        <f>E20+1</f>
+        <v>44696</v>
+      </c>
+      <c r="F21" s="85">
+        <f>E21</f>
+        <v>44696</v>
+      </c>
       <c r="G21" s="17"/>
-      <c r="H21" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
+      <c r="H21" s="17">
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="I21" s="44"/>
       <c r="J21" s="44"/>
@@ -3282,63 +2983,57 @@
       <c r="AA21" s="44"/>
       <c r="AB21" s="44"/>
       <c r="AC21" s="44"/>
-      <c r="AD21" s="44"/>
-      <c r="AE21" s="44"/>
-      <c r="AF21" s="44"/>
-      <c r="AG21" s="44"/>
-      <c r="AH21" s="44"/>
-      <c r="AI21" s="44"/>
-      <c r="AJ21" s="44"/>
-      <c r="AK21" s="44"/>
-      <c r="AL21" s="44"/>
-      <c r="AM21" s="44"/>
-      <c r="AN21" s="44"/>
-      <c r="AO21" s="44"/>
-      <c r="AP21" s="44"/>
-      <c r="AQ21" s="44"/>
-      <c r="AR21" s="44"/>
-      <c r="AS21" s="44"/>
-      <c r="AT21" s="44"/>
-      <c r="AU21" s="44"/>
-      <c r="AV21" s="44"/>
-      <c r="AW21" s="44"/>
-      <c r="AX21" s="44"/>
-      <c r="AY21" s="44"/>
-      <c r="AZ21" s="44"/>
-      <c r="BA21" s="44"/>
-      <c r="BB21" s="44"/>
-      <c r="BC21" s="44"/>
-      <c r="BD21" s="44"/>
-      <c r="BE21" s="44"/>
-      <c r="BF21" s="44"/>
-      <c r="BG21" s="44"/>
-      <c r="BH21" s="44"/>
-      <c r="BI21" s="44"/>
-      <c r="BJ21" s="44"/>
-      <c r="BK21" s="44"/>
-      <c r="BL21" s="44"/>
+      <c r="AD21"/>
+      <c r="AE21"/>
+      <c r="AF21"/>
+      <c r="AG21"/>
+      <c r="AH21"/>
+      <c r="AI21"/>
+      <c r="AJ21"/>
+      <c r="AK21"/>
+      <c r="AL21"/>
+      <c r="AM21"/>
+      <c r="AN21"/>
+      <c r="AO21"/>
+      <c r="AP21"/>
+      <c r="AQ21"/>
+      <c r="AR21"/>
+      <c r="AS21"/>
+      <c r="AT21"/>
+      <c r="AU21"/>
+      <c r="AV21"/>
+      <c r="AW21"/>
+      <c r="AX21"/>
+      <c r="AY21"/>
+      <c r="AZ21"/>
+      <c r="BA21"/>
+      <c r="BB21"/>
+      <c r="BC21"/>
+      <c r="BD21"/>
+      <c r="BE21"/>
+      <c r="BF21"/>
+      <c r="BG21"/>
+      <c r="BH21"/>
+      <c r="BI21"/>
+      <c r="BJ21"/>
+      <c r="BK21"/>
+      <c r="BL21"/>
     </row>
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="58"/>
-      <c r="B22" s="77" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="71" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="32"/>
-      <c r="E22" s="86">
-        <f>F20+1</f>
-        <v>44697</v>
-      </c>
-      <c r="F22" s="86">
-        <f>E22+2</f>
-        <v>44699</v>
-      </c>
+      <c r="A22" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="70"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="31"/>
       <c r="G22" s="17"/>
-      <c r="H22" s="17">
-        <f t="shared" si="6"/>
-        <v>3</v>
+      <c r="H22" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="I22" s="44"/>
       <c r="J22" s="44"/>
@@ -3361,63 +3056,63 @@
       <c r="AA22" s="44"/>
       <c r="AB22" s="44"/>
       <c r="AC22" s="44"/>
-      <c r="AD22" s="44"/>
-      <c r="AE22" s="44"/>
-      <c r="AF22" s="44"/>
-      <c r="AG22" s="44"/>
-      <c r="AH22" s="44"/>
-      <c r="AI22" s="44"/>
-      <c r="AJ22" s="44"/>
-      <c r="AK22" s="44"/>
-      <c r="AL22" s="44"/>
-      <c r="AM22" s="44"/>
-      <c r="AN22" s="44"/>
-      <c r="AO22" s="44"/>
-      <c r="AP22" s="44"/>
-      <c r="AQ22" s="44"/>
-      <c r="AR22" s="44"/>
-      <c r="AS22" s="44"/>
-      <c r="AT22" s="44"/>
-      <c r="AU22" s="44"/>
-      <c r="AV22" s="44"/>
-      <c r="AW22" s="44"/>
-      <c r="AX22" s="44"/>
-      <c r="AY22" s="44"/>
-      <c r="AZ22" s="44"/>
-      <c r="BA22" s="44"/>
-      <c r="BB22" s="44"/>
-      <c r="BC22" s="44"/>
-      <c r="BD22" s="44"/>
-      <c r="BE22" s="44"/>
-      <c r="BF22" s="44"/>
-      <c r="BG22" s="44"/>
-      <c r="BH22" s="44"/>
-      <c r="BI22" s="44"/>
-      <c r="BJ22" s="44"/>
-      <c r="BK22" s="44"/>
-      <c r="BL22" s="44"/>
+      <c r="AD22"/>
+      <c r="AE22"/>
+      <c r="AF22"/>
+      <c r="AG22"/>
+      <c r="AH22"/>
+      <c r="AI22"/>
+      <c r="AJ22"/>
+      <c r="AK22"/>
+      <c r="AL22"/>
+      <c r="AM22"/>
+      <c r="AN22"/>
+      <c r="AO22"/>
+      <c r="AP22"/>
+      <c r="AQ22"/>
+      <c r="AR22"/>
+      <c r="AS22"/>
+      <c r="AT22"/>
+      <c r="AU22"/>
+      <c r="AV22"/>
+      <c r="AW22"/>
+      <c r="AX22"/>
+      <c r="AY22"/>
+      <c r="AZ22"/>
+      <c r="BA22"/>
+      <c r="BB22"/>
+      <c r="BC22"/>
+      <c r="BD22"/>
+      <c r="BE22"/>
+      <c r="BF22"/>
+      <c r="BG22"/>
+      <c r="BH22"/>
+      <c r="BI22"/>
+      <c r="BJ22"/>
+      <c r="BK22"/>
+      <c r="BL22"/>
     </row>
     <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="58"/>
       <c r="B23" s="77" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="C23" s="71" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D23" s="32"/>
       <c r="E23" s="86">
-        <f>F22+1</f>
-        <v>44700</v>
+        <f>F21+2</f>
+        <v>44698</v>
       </c>
       <c r="F23" s="86">
-        <f>E23+2</f>
-        <v>44702</v>
+        <f>E23</f>
+        <v>44698</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="17">
-        <f t="shared" si="6"/>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="I23" s="44"/>
       <c r="J23" s="44"/>
@@ -3440,63 +3135,63 @@
       <c r="AA23" s="44"/>
       <c r="AB23" s="44"/>
       <c r="AC23" s="44"/>
-      <c r="AD23" s="44"/>
-      <c r="AE23" s="44"/>
-      <c r="AF23" s="44"/>
-      <c r="AG23" s="44"/>
-      <c r="AH23" s="44"/>
-      <c r="AI23" s="44"/>
-      <c r="AJ23" s="44"/>
-      <c r="AK23" s="44"/>
-      <c r="AL23" s="44"/>
-      <c r="AM23" s="44"/>
-      <c r="AN23" s="44"/>
-      <c r="AO23" s="44"/>
-      <c r="AP23" s="44"/>
-      <c r="AQ23" s="44"/>
-      <c r="AR23" s="44"/>
-      <c r="AS23" s="44"/>
-      <c r="AT23" s="44"/>
-      <c r="AU23" s="44"/>
-      <c r="AV23" s="44"/>
-      <c r="AW23" s="44"/>
-      <c r="AX23" s="44"/>
-      <c r="AY23" s="44"/>
-      <c r="AZ23" s="44"/>
-      <c r="BA23" s="44"/>
-      <c r="BB23" s="44"/>
-      <c r="BC23" s="44"/>
-      <c r="BD23" s="44"/>
-      <c r="BE23" s="44"/>
-      <c r="BF23" s="44"/>
-      <c r="BG23" s="44"/>
-      <c r="BH23" s="44"/>
-      <c r="BI23" s="44"/>
-      <c r="BJ23" s="44"/>
-      <c r="BK23" s="44"/>
-      <c r="BL23" s="44"/>
+      <c r="AD23"/>
+      <c r="AE23"/>
+      <c r="AF23"/>
+      <c r="AG23"/>
+      <c r="AH23"/>
+      <c r="AI23"/>
+      <c r="AJ23"/>
+      <c r="AK23"/>
+      <c r="AL23"/>
+      <c r="AM23"/>
+      <c r="AN23"/>
+      <c r="AO23"/>
+      <c r="AP23"/>
+      <c r="AQ23"/>
+      <c r="AR23"/>
+      <c r="AS23"/>
+      <c r="AT23"/>
+      <c r="AU23"/>
+      <c r="AV23"/>
+      <c r="AW23"/>
+      <c r="AX23"/>
+      <c r="AY23"/>
+      <c r="AZ23"/>
+      <c r="BA23"/>
+      <c r="BB23"/>
+      <c r="BC23"/>
+      <c r="BD23"/>
+      <c r="BE23"/>
+      <c r="BF23"/>
+      <c r="BG23"/>
+      <c r="BH23"/>
+      <c r="BI23"/>
+      <c r="BJ23"/>
+      <c r="BK23"/>
+      <c r="BL23"/>
     </row>
     <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="58"/>
       <c r="B24" s="77" t="s">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="C24" s="71" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D24" s="32"/>
       <c r="E24" s="86">
-        <f>F23</f>
-        <v>44702</v>
+        <f>F23+1</f>
+        <v>44699</v>
       </c>
       <c r="F24" s="86">
-        <f>E24+2</f>
-        <v>44704</v>
+        <f>E24</f>
+        <v>44699</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="17">
-        <f t="shared" si="6"/>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="I24" s="44"/>
       <c r="J24" s="44"/>
@@ -3519,63 +3214,63 @@
       <c r="AA24" s="44"/>
       <c r="AB24" s="44"/>
       <c r="AC24" s="44"/>
-      <c r="AD24" s="44"/>
-      <c r="AE24" s="44"/>
-      <c r="AF24" s="44"/>
-      <c r="AG24" s="44"/>
-      <c r="AH24" s="44"/>
-      <c r="AI24" s="44"/>
-      <c r="AJ24" s="44"/>
-      <c r="AK24" s="44"/>
-      <c r="AL24" s="44"/>
-      <c r="AM24" s="44"/>
-      <c r="AN24" s="44"/>
-      <c r="AO24" s="44"/>
-      <c r="AP24" s="44"/>
-      <c r="AQ24" s="44"/>
-      <c r="AR24" s="44"/>
-      <c r="AS24" s="44"/>
-      <c r="AT24" s="44"/>
-      <c r="AU24" s="44"/>
-      <c r="AV24" s="44"/>
-      <c r="AW24" s="44"/>
-      <c r="AX24" s="44"/>
-      <c r="AY24" s="44"/>
-      <c r="AZ24" s="44"/>
-      <c r="BA24" s="44"/>
-      <c r="BB24" s="44"/>
-      <c r="BC24" s="44"/>
-      <c r="BD24" s="44"/>
-      <c r="BE24" s="44"/>
-      <c r="BF24" s="44"/>
-      <c r="BG24" s="44"/>
-      <c r="BH24" s="44"/>
-      <c r="BI24" s="44"/>
-      <c r="BJ24" s="44"/>
-      <c r="BK24" s="44"/>
-      <c r="BL24" s="44"/>
+      <c r="AD24"/>
+      <c r="AE24"/>
+      <c r="AF24"/>
+      <c r="AG24"/>
+      <c r="AH24"/>
+      <c r="AI24"/>
+      <c r="AJ24"/>
+      <c r="AK24"/>
+      <c r="AL24"/>
+      <c r="AM24"/>
+      <c r="AN24"/>
+      <c r="AO24"/>
+      <c r="AP24"/>
+      <c r="AQ24"/>
+      <c r="AR24"/>
+      <c r="AS24"/>
+      <c r="AT24"/>
+      <c r="AU24"/>
+      <c r="AV24"/>
+      <c r="AW24"/>
+      <c r="AX24"/>
+      <c r="AY24"/>
+      <c r="AZ24"/>
+      <c r="BA24"/>
+      <c r="BB24"/>
+      <c r="BC24"/>
+      <c r="BD24"/>
+      <c r="BE24"/>
+      <c r="BF24"/>
+      <c r="BG24"/>
+      <c r="BH24"/>
+      <c r="BI24"/>
+      <c r="BJ24"/>
+      <c r="BK24"/>
+      <c r="BL24"/>
     </row>
     <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="58"/>
       <c r="B25" s="77" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C25" s="71" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D25" s="32"/>
       <c r="E25" s="86">
-        <f>E24+1</f>
-        <v>44703</v>
+        <f>F24</f>
+        <v>44699</v>
       </c>
       <c r="F25" s="86">
-        <f>E25+3</f>
-        <v>44706</v>
+        <f>E25+1</f>
+        <v>44700</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="17">
-        <f t="shared" si="6"/>
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="I25" s="44"/>
       <c r="J25" s="44"/>
@@ -3598,63 +3293,63 @@
       <c r="AA25" s="44"/>
       <c r="AB25" s="44"/>
       <c r="AC25" s="44"/>
-      <c r="AD25" s="44"/>
-      <c r="AE25" s="44"/>
-      <c r="AF25" s="44"/>
-      <c r="AG25" s="44"/>
-      <c r="AH25" s="44"/>
-      <c r="AI25" s="44"/>
-      <c r="AJ25" s="44"/>
-      <c r="AK25" s="44"/>
-      <c r="AL25" s="44"/>
-      <c r="AM25" s="44"/>
-      <c r="AN25" s="44"/>
-      <c r="AO25" s="44"/>
-      <c r="AP25" s="44"/>
-      <c r="AQ25" s="44"/>
-      <c r="AR25" s="44"/>
-      <c r="AS25" s="44"/>
-      <c r="AT25" s="44"/>
-      <c r="AU25" s="44"/>
-      <c r="AV25" s="44"/>
-      <c r="AW25" s="44"/>
-      <c r="AX25" s="44"/>
-      <c r="AY25" s="44"/>
-      <c r="AZ25" s="44"/>
-      <c r="BA25" s="44"/>
-      <c r="BB25" s="44"/>
-      <c r="BC25" s="44"/>
-      <c r="BD25" s="44"/>
-      <c r="BE25" s="44"/>
-      <c r="BF25" s="44"/>
-      <c r="BG25" s="44"/>
-      <c r="BH25" s="44"/>
-      <c r="BI25" s="44"/>
-      <c r="BJ25" s="44"/>
-      <c r="BK25" s="44"/>
-      <c r="BL25" s="44"/>
+      <c r="AD25"/>
+      <c r="AE25"/>
+      <c r="AF25"/>
+      <c r="AG25"/>
+      <c r="AH25"/>
+      <c r="AI25"/>
+      <c r="AJ25"/>
+      <c r="AK25"/>
+      <c r="AL25"/>
+      <c r="AM25"/>
+      <c r="AN25"/>
+      <c r="AO25"/>
+      <c r="AP25"/>
+      <c r="AQ25"/>
+      <c r="AR25"/>
+      <c r="AS25"/>
+      <c r="AT25"/>
+      <c r="AU25"/>
+      <c r="AV25"/>
+      <c r="AW25"/>
+      <c r="AX25"/>
+      <c r="AY25"/>
+      <c r="AZ25"/>
+      <c r="BA25"/>
+      <c r="BB25"/>
+      <c r="BC25"/>
+      <c r="BD25"/>
+      <c r="BE25"/>
+      <c r="BF25"/>
+      <c r="BG25"/>
+      <c r="BH25"/>
+      <c r="BI25"/>
+      <c r="BJ25"/>
+      <c r="BK25"/>
+      <c r="BL25"/>
     </row>
     <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="58"/>
       <c r="B26" s="77" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="C26" s="71" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D26" s="32"/>
       <c r="E26" s="86">
-        <f>E24</f>
-        <v>44702</v>
+        <f>E25+1</f>
+        <v>44700</v>
       </c>
       <c r="F26" s="86">
-        <f>E26+3</f>
-        <v>44705</v>
+        <f>E26</f>
+        <v>44700</v>
       </c>
       <c r="G26" s="17"/>
       <c r="H26" s="17">
-        <f t="shared" si="6"/>
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="I26" s="44"/>
       <c r="J26" s="44"/>
@@ -3677,57 +3372,63 @@
       <c r="AA26" s="44"/>
       <c r="AB26" s="44"/>
       <c r="AC26" s="44"/>
-      <c r="AD26" s="44"/>
-      <c r="AE26" s="44"/>
-      <c r="AF26" s="44"/>
-      <c r="AG26" s="44"/>
-      <c r="AH26" s="44"/>
-      <c r="AI26" s="44"/>
-      <c r="AJ26" s="44"/>
-      <c r="AK26" s="44"/>
-      <c r="AL26" s="44"/>
-      <c r="AM26" s="44"/>
-      <c r="AN26" s="44"/>
-      <c r="AO26" s="44"/>
-      <c r="AP26" s="44"/>
-      <c r="AQ26" s="44"/>
-      <c r="AR26" s="44"/>
-      <c r="AS26" s="44"/>
-      <c r="AT26" s="44"/>
-      <c r="AU26" s="44"/>
-      <c r="AV26" s="44"/>
-      <c r="AW26" s="44"/>
-      <c r="AX26" s="44"/>
-      <c r="AY26" s="44"/>
-      <c r="AZ26" s="44"/>
-      <c r="BA26" s="44"/>
-      <c r="BB26" s="44"/>
-      <c r="BC26" s="44"/>
-      <c r="BD26" s="44"/>
-      <c r="BE26" s="44"/>
-      <c r="BF26" s="44"/>
-      <c r="BG26" s="44"/>
-      <c r="BH26" s="44"/>
-      <c r="BI26" s="44"/>
-      <c r="BJ26" s="44"/>
-      <c r="BK26" s="44"/>
-      <c r="BL26" s="44"/>
+      <c r="AD26"/>
+      <c r="AE26"/>
+      <c r="AF26"/>
+      <c r="AG26"/>
+      <c r="AH26"/>
+      <c r="AI26"/>
+      <c r="AJ26"/>
+      <c r="AK26"/>
+      <c r="AL26"/>
+      <c r="AM26"/>
+      <c r="AN26"/>
+      <c r="AO26"/>
+      <c r="AP26"/>
+      <c r="AQ26"/>
+      <c r="AR26"/>
+      <c r="AS26"/>
+      <c r="AT26"/>
+      <c r="AU26"/>
+      <c r="AV26"/>
+      <c r="AW26"/>
+      <c r="AX26"/>
+      <c r="AY26"/>
+      <c r="AZ26"/>
+      <c r="BA26"/>
+      <c r="BB26"/>
+      <c r="BC26"/>
+      <c r="BD26"/>
+      <c r="BE26"/>
+      <c r="BF26"/>
+      <c r="BG26"/>
+      <c r="BH26"/>
+      <c r="BI26"/>
+      <c r="BJ26"/>
+      <c r="BK26"/>
+      <c r="BL26"/>
     </row>
     <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="72"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="36"/>
+      <c r="A27" s="58"/>
+      <c r="B27" s="77" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="71" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="32"/>
+      <c r="E27" s="86">
+        <f>F26</f>
+        <v>44700</v>
+      </c>
+      <c r="F27" s="86">
+        <f>E27+1</f>
+        <v>44701</v>
+      </c>
       <c r="G27" s="17"/>
-      <c r="H27" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
+      <c r="H27" s="17">
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="I27" s="44"/>
       <c r="J27" s="44"/>
@@ -3750,61 +3451,57 @@
       <c r="AA27" s="44"/>
       <c r="AB27" s="44"/>
       <c r="AC27" s="44"/>
-      <c r="AD27" s="44"/>
-      <c r="AE27" s="44"/>
-      <c r="AF27" s="44"/>
-      <c r="AG27" s="44"/>
-      <c r="AH27" s="44"/>
-      <c r="AI27" s="44"/>
-      <c r="AJ27" s="44"/>
-      <c r="AK27" s="44"/>
-      <c r="AL27" s="44"/>
-      <c r="AM27" s="44"/>
-      <c r="AN27" s="44"/>
-      <c r="AO27" s="44"/>
-      <c r="AP27" s="44"/>
-      <c r="AQ27" s="44"/>
-      <c r="AR27" s="44"/>
-      <c r="AS27" s="44"/>
-      <c r="AT27" s="44"/>
-      <c r="AU27" s="44"/>
-      <c r="AV27" s="44"/>
-      <c r="AW27" s="44"/>
-      <c r="AX27" s="44"/>
-      <c r="AY27" s="44"/>
-      <c r="AZ27" s="44"/>
-      <c r="BA27" s="44"/>
-      <c r="BB27" s="44"/>
-      <c r="BC27" s="44"/>
-      <c r="BD27" s="44"/>
-      <c r="BE27" s="44"/>
-      <c r="BF27" s="44"/>
-      <c r="BG27" s="44"/>
-      <c r="BH27" s="44"/>
-      <c r="BI27" s="44"/>
-      <c r="BJ27" s="44"/>
-      <c r="BK27" s="44"/>
-      <c r="BL27" s="44"/>
+      <c r="AD27"/>
+      <c r="AE27"/>
+      <c r="AF27"/>
+      <c r="AG27"/>
+      <c r="AH27"/>
+      <c r="AI27"/>
+      <c r="AJ27"/>
+      <c r="AK27"/>
+      <c r="AL27"/>
+      <c r="AM27"/>
+      <c r="AN27"/>
+      <c r="AO27"/>
+      <c r="AP27"/>
+      <c r="AQ27"/>
+      <c r="AR27"/>
+      <c r="AS27"/>
+      <c r="AT27"/>
+      <c r="AU27"/>
+      <c r="AV27"/>
+      <c r="AW27"/>
+      <c r="AX27"/>
+      <c r="AY27"/>
+      <c r="AZ27"/>
+      <c r="BA27"/>
+      <c r="BB27"/>
+      <c r="BC27"/>
+      <c r="BD27"/>
+      <c r="BE27"/>
+      <c r="BF27"/>
+      <c r="BG27"/>
+      <c r="BH27"/>
+      <c r="BI27"/>
+      <c r="BJ27"/>
+      <c r="BK27"/>
+      <c r="BL27"/>
     </row>
     <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="58"/>
-      <c r="B28" s="78" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="73" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="37"/>
-      <c r="E28" s="87" t="s">
-        <v>30</v>
-      </c>
-      <c r="F28" s="87" t="s">
-        <v>30</v>
-      </c>
+      <c r="A28" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="72"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="36"/>
       <c r="G28" s="17"/>
-      <c r="H28" s="17" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="H28" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="I28" s="44"/>
       <c r="J28" s="44"/>
@@ -3827,61 +3524,63 @@
       <c r="AA28" s="44"/>
       <c r="AB28" s="44"/>
       <c r="AC28" s="44"/>
-      <c r="AD28" s="44"/>
-      <c r="AE28" s="44"/>
-      <c r="AF28" s="44"/>
-      <c r="AG28" s="44"/>
-      <c r="AH28" s="44"/>
-      <c r="AI28" s="44"/>
-      <c r="AJ28" s="44"/>
-      <c r="AK28" s="44"/>
-      <c r="AL28" s="44"/>
-      <c r="AM28" s="44"/>
-      <c r="AN28" s="44"/>
-      <c r="AO28" s="44"/>
-      <c r="AP28" s="44"/>
-      <c r="AQ28" s="44"/>
-      <c r="AR28" s="44"/>
-      <c r="AS28" s="44"/>
-      <c r="AT28" s="44"/>
-      <c r="AU28" s="44"/>
-      <c r="AV28" s="44"/>
-      <c r="AW28" s="44"/>
-      <c r="AX28" s="44"/>
-      <c r="AY28" s="44"/>
-      <c r="AZ28" s="44"/>
-      <c r="BA28" s="44"/>
-      <c r="BB28" s="44"/>
-      <c r="BC28" s="44"/>
-      <c r="BD28" s="44"/>
-      <c r="BE28" s="44"/>
-      <c r="BF28" s="44"/>
-      <c r="BG28" s="44"/>
-      <c r="BH28" s="44"/>
-      <c r="BI28" s="44"/>
-      <c r="BJ28" s="44"/>
-      <c r="BK28" s="44"/>
-      <c r="BL28" s="44"/>
+      <c r="AD28"/>
+      <c r="AE28"/>
+      <c r="AF28"/>
+      <c r="AG28"/>
+      <c r="AH28"/>
+      <c r="AI28"/>
+      <c r="AJ28"/>
+      <c r="AK28"/>
+      <c r="AL28"/>
+      <c r="AM28"/>
+      <c r="AN28"/>
+      <c r="AO28"/>
+      <c r="AP28"/>
+      <c r="AQ28"/>
+      <c r="AR28"/>
+      <c r="AS28"/>
+      <c r="AT28"/>
+      <c r="AU28"/>
+      <c r="AV28"/>
+      <c r="AW28"/>
+      <c r="AX28"/>
+      <c r="AY28"/>
+      <c r="AZ28"/>
+      <c r="BA28"/>
+      <c r="BB28"/>
+      <c r="BC28"/>
+      <c r="BD28"/>
+      <c r="BE28"/>
+      <c r="BF28"/>
+      <c r="BG28"/>
+      <c r="BH28"/>
+      <c r="BI28"/>
+      <c r="BJ28"/>
+      <c r="BK28"/>
+      <c r="BL28"/>
     </row>
     <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="58"/>
       <c r="B29" s="78" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="C29" s="73" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D29" s="37"/>
-      <c r="E29" s="87" t="s">
-        <v>30</v>
-      </c>
-      <c r="F29" s="87" t="s">
-        <v>30</v>
+      <c r="E29" s="87">
+        <f>F27</f>
+        <v>44701</v>
+      </c>
+      <c r="F29" s="87">
+        <f>E29</f>
+        <v>44701</v>
       </c>
       <c r="G29" s="17"/>
-      <c r="H29" s="17" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="H29" s="17">
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="I29" s="44"/>
       <c r="J29" s="44"/>
@@ -3904,61 +3603,63 @@
       <c r="AA29" s="44"/>
       <c r="AB29" s="44"/>
       <c r="AC29" s="44"/>
-      <c r="AD29" s="44"/>
-      <c r="AE29" s="44"/>
-      <c r="AF29" s="44"/>
-      <c r="AG29" s="44"/>
-      <c r="AH29" s="44"/>
-      <c r="AI29" s="44"/>
-      <c r="AJ29" s="44"/>
-      <c r="AK29" s="44"/>
-      <c r="AL29" s="44"/>
-      <c r="AM29" s="44"/>
-      <c r="AN29" s="44"/>
-      <c r="AO29" s="44"/>
-      <c r="AP29" s="44"/>
-      <c r="AQ29" s="44"/>
-      <c r="AR29" s="44"/>
-      <c r="AS29" s="44"/>
-      <c r="AT29" s="44"/>
-      <c r="AU29" s="44"/>
-      <c r="AV29" s="44"/>
-      <c r="AW29" s="44"/>
-      <c r="AX29" s="44"/>
-      <c r="AY29" s="44"/>
-      <c r="AZ29" s="44"/>
-      <c r="BA29" s="44"/>
-      <c r="BB29" s="44"/>
-      <c r="BC29" s="44"/>
-      <c r="BD29" s="44"/>
-      <c r="BE29" s="44"/>
-      <c r="BF29" s="44"/>
-      <c r="BG29" s="44"/>
-      <c r="BH29" s="44"/>
-      <c r="BI29" s="44"/>
-      <c r="BJ29" s="44"/>
-      <c r="BK29" s="44"/>
-      <c r="BL29" s="44"/>
+      <c r="AD29"/>
+      <c r="AE29"/>
+      <c r="AF29"/>
+      <c r="AG29"/>
+      <c r="AH29"/>
+      <c r="AI29"/>
+      <c r="AJ29"/>
+      <c r="AK29"/>
+      <c r="AL29"/>
+      <c r="AM29"/>
+      <c r="AN29"/>
+      <c r="AO29"/>
+      <c r="AP29"/>
+      <c r="AQ29"/>
+      <c r="AR29"/>
+      <c r="AS29"/>
+      <c r="AT29"/>
+      <c r="AU29"/>
+      <c r="AV29"/>
+      <c r="AW29"/>
+      <c r="AX29"/>
+      <c r="AY29"/>
+      <c r="AZ29"/>
+      <c r="BA29"/>
+      <c r="BB29"/>
+      <c r="BC29"/>
+      <c r="BD29"/>
+      <c r="BE29"/>
+      <c r="BF29"/>
+      <c r="BG29"/>
+      <c r="BH29"/>
+      <c r="BI29"/>
+      <c r="BJ29"/>
+      <c r="BK29"/>
+      <c r="BL29"/>
     </row>
     <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="58"/>
       <c r="B30" s="78" t="s">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="C30" s="73" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D30" s="37"/>
-      <c r="E30" s="87" t="s">
-        <v>30</v>
-      </c>
-      <c r="F30" s="87" t="s">
-        <v>30</v>
+      <c r="E30" s="87">
+        <f>F29</f>
+        <v>44701</v>
+      </c>
+      <c r="F30" s="87">
+        <f>E30+1</f>
+        <v>44702</v>
       </c>
       <c r="G30" s="17"/>
-      <c r="H30" s="17" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="H30" s="17">
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="I30" s="44"/>
       <c r="J30" s="44"/>
@@ -3981,61 +3682,63 @@
       <c r="AA30" s="44"/>
       <c r="AB30" s="44"/>
       <c r="AC30" s="44"/>
-      <c r="AD30" s="44"/>
-      <c r="AE30" s="44"/>
-      <c r="AF30" s="44"/>
-      <c r="AG30" s="44"/>
-      <c r="AH30" s="44"/>
-      <c r="AI30" s="44"/>
-      <c r="AJ30" s="44"/>
-      <c r="AK30" s="44"/>
-      <c r="AL30" s="44"/>
-      <c r="AM30" s="44"/>
-      <c r="AN30" s="44"/>
-      <c r="AO30" s="44"/>
-      <c r="AP30" s="44"/>
-      <c r="AQ30" s="44"/>
-      <c r="AR30" s="44"/>
-      <c r="AS30" s="44"/>
-      <c r="AT30" s="44"/>
-      <c r="AU30" s="44"/>
-      <c r="AV30" s="44"/>
-      <c r="AW30" s="44"/>
-      <c r="AX30" s="44"/>
-      <c r="AY30" s="44"/>
-      <c r="AZ30" s="44"/>
-      <c r="BA30" s="44"/>
-      <c r="BB30" s="44"/>
-      <c r="BC30" s="44"/>
-      <c r="BD30" s="44"/>
-      <c r="BE30" s="44"/>
-      <c r="BF30" s="44"/>
-      <c r="BG30" s="44"/>
-      <c r="BH30" s="44"/>
-      <c r="BI30" s="44"/>
-      <c r="BJ30" s="44"/>
-      <c r="BK30" s="44"/>
-      <c r="BL30" s="44"/>
+      <c r="AD30"/>
+      <c r="AE30"/>
+      <c r="AF30"/>
+      <c r="AG30"/>
+      <c r="AH30"/>
+      <c r="AI30"/>
+      <c r="AJ30"/>
+      <c r="AK30"/>
+      <c r="AL30"/>
+      <c r="AM30"/>
+      <c r="AN30"/>
+      <c r="AO30"/>
+      <c r="AP30"/>
+      <c r="AQ30"/>
+      <c r="AR30"/>
+      <c r="AS30"/>
+      <c r="AT30"/>
+      <c r="AU30"/>
+      <c r="AV30"/>
+      <c r="AW30"/>
+      <c r="AX30"/>
+      <c r="AY30"/>
+      <c r="AZ30"/>
+      <c r="BA30"/>
+      <c r="BB30"/>
+      <c r="BC30"/>
+      <c r="BD30"/>
+      <c r="BE30"/>
+      <c r="BF30"/>
+      <c r="BG30"/>
+      <c r="BH30"/>
+      <c r="BI30"/>
+      <c r="BJ30"/>
+      <c r="BK30"/>
+      <c r="BL30"/>
     </row>
     <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="58"/>
       <c r="B31" s="78" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="37"/>
+      <c r="E31" s="87">
+        <f>F30</f>
+        <v>44702</v>
+      </c>
+      <c r="F31" s="87">
+        <f>F30</f>
+        <v>44702</v>
+      </c>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17">
+        <f t="shared" si="3"/>
         <v>1</v>
-      </c>
-      <c r="C31" s="73" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="37"/>
-      <c r="E31" s="87" t="s">
-        <v>30</v>
-      </c>
-      <c r="F31" s="87" t="s">
-        <v>30</v>
-      </c>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
       </c>
       <c r="I31" s="44"/>
       <c r="J31" s="44"/>
@@ -4058,61 +3761,63 @@
       <c r="AA31" s="44"/>
       <c r="AB31" s="44"/>
       <c r="AC31" s="44"/>
-      <c r="AD31" s="44"/>
-      <c r="AE31" s="44"/>
-      <c r="AF31" s="44"/>
-      <c r="AG31" s="44"/>
-      <c r="AH31" s="44"/>
-      <c r="AI31" s="44"/>
-      <c r="AJ31" s="44"/>
-      <c r="AK31" s="44"/>
-      <c r="AL31" s="44"/>
-      <c r="AM31" s="44"/>
-      <c r="AN31" s="44"/>
-      <c r="AO31" s="44"/>
-      <c r="AP31" s="44"/>
-      <c r="AQ31" s="44"/>
-      <c r="AR31" s="44"/>
-      <c r="AS31" s="44"/>
-      <c r="AT31" s="44"/>
-      <c r="AU31" s="44"/>
-      <c r="AV31" s="44"/>
-      <c r="AW31" s="44"/>
-      <c r="AX31" s="44"/>
-      <c r="AY31" s="44"/>
-      <c r="AZ31" s="44"/>
-      <c r="BA31" s="44"/>
-      <c r="BB31" s="44"/>
-      <c r="BC31" s="44"/>
-      <c r="BD31" s="44"/>
-      <c r="BE31" s="44"/>
-      <c r="BF31" s="44"/>
-      <c r="BG31" s="44"/>
-      <c r="BH31" s="44"/>
-      <c r="BI31" s="44"/>
-      <c r="BJ31" s="44"/>
-      <c r="BK31" s="44"/>
-      <c r="BL31" s="44"/>
+      <c r="AD31"/>
+      <c r="AE31"/>
+      <c r="AF31"/>
+      <c r="AG31"/>
+      <c r="AH31"/>
+      <c r="AI31"/>
+      <c r="AJ31"/>
+      <c r="AK31"/>
+      <c r="AL31"/>
+      <c r="AM31"/>
+      <c r="AN31"/>
+      <c r="AO31"/>
+      <c r="AP31"/>
+      <c r="AQ31"/>
+      <c r="AR31"/>
+      <c r="AS31"/>
+      <c r="AT31"/>
+      <c r="AU31"/>
+      <c r="AV31"/>
+      <c r="AW31"/>
+      <c r="AX31"/>
+      <c r="AY31"/>
+      <c r="AZ31"/>
+      <c r="BA31"/>
+      <c r="BB31"/>
+      <c r="BC31"/>
+      <c r="BD31"/>
+      <c r="BE31"/>
+      <c r="BF31"/>
+      <c r="BG31"/>
+      <c r="BH31"/>
+      <c r="BI31"/>
+      <c r="BJ31"/>
+      <c r="BK31"/>
+      <c r="BL31"/>
     </row>
     <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="58"/>
       <c r="B32" s="78" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="37"/>
+      <c r="E32" s="87">
+        <f>F31+1</f>
+        <v>44703</v>
+      </c>
+      <c r="F32" s="87">
+        <f>E32+1</f>
+        <v>44704</v>
+      </c>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17">
+        <f t="shared" si="3"/>
         <v>2</v>
-      </c>
-      <c r="C32" s="73" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="37"/>
-      <c r="E32" s="87" t="s">
-        <v>30</v>
-      </c>
-      <c r="F32" s="87" t="s">
-        <v>30</v>
-      </c>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
       </c>
       <c r="I32" s="44"/>
       <c r="J32" s="44"/>
@@ -4135,56 +3840,61 @@
       <c r="AA32" s="44"/>
       <c r="AB32" s="44"/>
       <c r="AC32" s="44"/>
-      <c r="AD32" s="44"/>
-      <c r="AE32" s="44"/>
-      <c r="AF32" s="44"/>
-      <c r="AG32" s="44"/>
-      <c r="AH32" s="44"/>
-      <c r="AI32" s="44"/>
-      <c r="AJ32" s="44"/>
-      <c r="AK32" s="44"/>
-      <c r="AL32" s="44"/>
-      <c r="AM32" s="44"/>
-      <c r="AN32" s="44"/>
-      <c r="AO32" s="44"/>
-      <c r="AP32" s="44"/>
-      <c r="AQ32" s="44"/>
-      <c r="AR32" s="44"/>
-      <c r="AS32" s="44"/>
-      <c r="AT32" s="44"/>
-      <c r="AU32" s="44"/>
-      <c r="AV32" s="44"/>
-      <c r="AW32" s="44"/>
-      <c r="AX32" s="44"/>
-      <c r="AY32" s="44"/>
-      <c r="AZ32" s="44"/>
-      <c r="BA32" s="44"/>
-      <c r="BB32" s="44"/>
-      <c r="BC32" s="44"/>
-      <c r="BD32" s="44"/>
-      <c r="BE32" s="44"/>
-      <c r="BF32" s="44"/>
-      <c r="BG32" s="44"/>
-      <c r="BH32" s="44"/>
-      <c r="BI32" s="44"/>
-      <c r="BJ32" s="44"/>
-      <c r="BK32" s="44"/>
-      <c r="BL32" s="44"/>
+      <c r="AD32"/>
+      <c r="AE32"/>
+      <c r="AF32"/>
+      <c r="AG32"/>
+      <c r="AH32"/>
+      <c r="AI32"/>
+      <c r="AJ32"/>
+      <c r="AK32"/>
+      <c r="AL32"/>
+      <c r="AM32"/>
+      <c r="AN32"/>
+      <c r="AO32"/>
+      <c r="AP32"/>
+      <c r="AQ32"/>
+      <c r="AR32"/>
+      <c r="AS32"/>
+      <c r="AT32"/>
+      <c r="AU32"/>
+      <c r="AV32"/>
+      <c r="AW32"/>
+      <c r="AX32"/>
+      <c r="AY32"/>
+      <c r="AZ32"/>
+      <c r="BA32"/>
+      <c r="BB32"/>
+      <c r="BC32"/>
+      <c r="BD32"/>
+      <c r="BE32"/>
+      <c r="BF32"/>
+      <c r="BG32"/>
+      <c r="BH32"/>
+      <c r="BI32"/>
+      <c r="BJ32"/>
+      <c r="BK32"/>
+      <c r="BL32"/>
     </row>
     <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="58" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="79"/>
-      <c r="C33" s="74"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="65"/>
-      <c r="F33" s="65"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="78" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="37"/>
+      <c r="E33" s="87">
+        <f>F32</f>
+        <v>44704</v>
+      </c>
+      <c r="F33" s="87">
+        <f>E33+1</f>
+        <v>44705</v>
+      </c>
       <c r="G33" s="17"/>
-      <c r="H33" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
+      <c r="H33" s="17"/>
       <c r="I33" s="44"/>
       <c r="J33" s="44"/>
       <c r="K33" s="44"/>
@@ -4206,140 +3916,579 @@
       <c r="AA33" s="44"/>
       <c r="AB33" s="44"/>
       <c r="AC33" s="44"/>
-      <c r="AD33" s="44"/>
-      <c r="AE33" s="44"/>
-      <c r="AF33" s="44"/>
-      <c r="AG33" s="44"/>
-      <c r="AH33" s="44"/>
-      <c r="AI33" s="44"/>
-      <c r="AJ33" s="44"/>
-      <c r="AK33" s="44"/>
-      <c r="AL33" s="44"/>
-      <c r="AM33" s="44"/>
-      <c r="AN33" s="44"/>
-      <c r="AO33" s="44"/>
-      <c r="AP33" s="44"/>
-      <c r="AQ33" s="44"/>
-      <c r="AR33" s="44"/>
-      <c r="AS33" s="44"/>
-      <c r="AT33" s="44"/>
-      <c r="AU33" s="44"/>
-      <c r="AV33" s="44"/>
-      <c r="AW33" s="44"/>
-      <c r="AX33" s="44"/>
-      <c r="AY33" s="44"/>
-      <c r="AZ33" s="44"/>
-      <c r="BA33" s="44"/>
-      <c r="BB33" s="44"/>
-      <c r="BC33" s="44"/>
-      <c r="BD33" s="44"/>
-      <c r="BE33" s="44"/>
-      <c r="BF33" s="44"/>
-      <c r="BG33" s="44"/>
-      <c r="BH33" s="44"/>
-      <c r="BI33" s="44"/>
-      <c r="BJ33" s="44"/>
-      <c r="BK33" s="44"/>
-      <c r="BL33" s="44"/>
+      <c r="AD33"/>
+      <c r="AE33"/>
+      <c r="AF33"/>
+      <c r="AG33"/>
+      <c r="AH33"/>
+      <c r="AI33"/>
+      <c r="AJ33"/>
+      <c r="AK33"/>
+      <c r="AL33"/>
+      <c r="AM33"/>
+      <c r="AN33"/>
+      <c r="AO33"/>
+      <c r="AP33"/>
+      <c r="AQ33"/>
+      <c r="AR33"/>
+      <c r="AS33"/>
+      <c r="AT33"/>
+      <c r="AU33"/>
+      <c r="AV33"/>
+      <c r="AW33"/>
+      <c r="AX33"/>
+      <c r="AY33"/>
+      <c r="AZ33"/>
+      <c r="BA33"/>
+      <c r="BB33"/>
+      <c r="BC33"/>
+      <c r="BD33"/>
+      <c r="BE33"/>
+      <c r="BF33"/>
+      <c r="BG33"/>
+      <c r="BH33"/>
+      <c r="BI33"/>
+      <c r="BJ33"/>
+      <c r="BK33"/>
+      <c r="BL33"/>
     </row>
     <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="59" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="38" t="s">
+      <c r="A34" s="58"/>
+      <c r="B34" s="99" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="100"/>
+      <c r="D34" s="101"/>
+      <c r="E34" s="102"/>
+      <c r="F34" s="103"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="44"/>
+      <c r="L34" s="44"/>
+      <c r="M34" s="44"/>
+      <c r="N34" s="44"/>
+      <c r="O34" s="44"/>
+      <c r="P34" s="44"/>
+      <c r="Q34" s="44"/>
+      <c r="R34" s="44"/>
+      <c r="S34" s="44"/>
+      <c r="T34" s="44"/>
+      <c r="U34" s="44"/>
+      <c r="V34" s="44"/>
+      <c r="W34" s="44"/>
+      <c r="X34" s="44"/>
+      <c r="Y34" s="44"/>
+      <c r="Z34" s="44"/>
+      <c r="AA34" s="44"/>
+      <c r="AB34" s="44"/>
+      <c r="AC34" s="44"/>
+      <c r="AD34"/>
+      <c r="AE34"/>
+      <c r="AF34"/>
+      <c r="AG34"/>
+      <c r="AH34"/>
+      <c r="AI34"/>
+      <c r="AJ34"/>
+      <c r="AK34"/>
+      <c r="AL34"/>
+      <c r="AM34"/>
+      <c r="AN34"/>
+      <c r="AO34"/>
+      <c r="AP34"/>
+      <c r="AQ34"/>
+      <c r="AR34"/>
+      <c r="AS34"/>
+      <c r="AT34"/>
+      <c r="AU34"/>
+      <c r="AV34"/>
+      <c r="AW34"/>
+      <c r="AX34"/>
+      <c r="AY34"/>
+      <c r="AZ34"/>
+      <c r="BA34"/>
+      <c r="BB34"/>
+      <c r="BC34"/>
+      <c r="BD34"/>
+      <c r="BE34"/>
+      <c r="BF34"/>
+      <c r="BG34"/>
+      <c r="BH34"/>
+      <c r="BI34"/>
+      <c r="BJ34"/>
+      <c r="BK34"/>
+      <c r="BL34"/>
+    </row>
+    <row r="35" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="58"/>
+      <c r="B35" s="95" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="96" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="97"/>
+      <c r="E35" s="98">
+        <f>F33</f>
+        <v>44705</v>
+      </c>
+      <c r="F35" s="98">
+        <f>E35</f>
+        <v>44705</v>
+      </c>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="44"/>
+      <c r="L35" s="44"/>
+      <c r="M35" s="44"/>
+      <c r="N35" s="44"/>
+      <c r="O35" s="44"/>
+      <c r="P35" s="44"/>
+      <c r="Q35" s="44"/>
+      <c r="R35" s="44"/>
+      <c r="S35" s="44"/>
+      <c r="T35" s="44"/>
+      <c r="U35" s="44"/>
+      <c r="V35" s="44"/>
+      <c r="W35" s="44"/>
+      <c r="X35" s="44"/>
+      <c r="Y35" s="44"/>
+      <c r="Z35" s="44"/>
+      <c r="AA35" s="44"/>
+      <c r="AB35" s="44"/>
+      <c r="AC35" s="44"/>
+      <c r="AD35"/>
+      <c r="AE35"/>
+      <c r="AF35"/>
+      <c r="AG35"/>
+      <c r="AH35"/>
+      <c r="AI35"/>
+      <c r="AJ35"/>
+      <c r="AK35"/>
+      <c r="AL35"/>
+      <c r="AM35"/>
+      <c r="AN35"/>
+      <c r="AO35"/>
+      <c r="AP35"/>
+      <c r="AQ35"/>
+      <c r="AR35"/>
+      <c r="AS35"/>
+      <c r="AT35"/>
+      <c r="AU35"/>
+      <c r="AV35"/>
+      <c r="AW35"/>
+      <c r="AX35"/>
+      <c r="AY35"/>
+      <c r="AZ35"/>
+      <c r="BA35"/>
+      <c r="BB35"/>
+      <c r="BC35"/>
+      <c r="BD35"/>
+      <c r="BE35"/>
+      <c r="BF35"/>
+      <c r="BG35"/>
+      <c r="BH35"/>
+      <c r="BI35"/>
+      <c r="BJ35"/>
+      <c r="BK35"/>
+      <c r="BL35"/>
+    </row>
+    <row r="36" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="58"/>
+      <c r="B36" s="95" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="96" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="97"/>
+      <c r="E36" s="98">
+        <f>F35</f>
+        <v>44705</v>
+      </c>
+      <c r="F36" s="98">
+        <f>E36+1</f>
+        <v>44706</v>
+      </c>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="44"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="44"/>
+      <c r="L36" s="44"/>
+      <c r="M36" s="44"/>
+      <c r="N36" s="44"/>
+      <c r="O36" s="44"/>
+      <c r="P36" s="44"/>
+      <c r="Q36" s="44"/>
+      <c r="R36" s="44"/>
+      <c r="S36" s="44"/>
+      <c r="T36" s="44"/>
+      <c r="U36" s="44"/>
+      <c r="V36" s="44"/>
+      <c r="W36" s="44"/>
+      <c r="X36" s="44"/>
+      <c r="Y36" s="44"/>
+      <c r="Z36" s="44"/>
+      <c r="AA36" s="44"/>
+      <c r="AB36" s="44"/>
+      <c r="AC36" s="44"/>
+      <c r="AD36"/>
+      <c r="AE36"/>
+      <c r="AF36"/>
+      <c r="AG36"/>
+      <c r="AH36"/>
+      <c r="AI36"/>
+      <c r="AJ36"/>
+      <c r="AK36"/>
+      <c r="AL36"/>
+      <c r="AM36"/>
+      <c r="AN36"/>
+      <c r="AO36"/>
+      <c r="AP36"/>
+      <c r="AQ36"/>
+      <c r="AR36"/>
+      <c r="AS36"/>
+      <c r="AT36"/>
+      <c r="AU36"/>
+      <c r="AV36"/>
+      <c r="AW36"/>
+      <c r="AX36"/>
+      <c r="AY36"/>
+      <c r="AZ36"/>
+      <c r="BA36"/>
+      <c r="BB36"/>
+      <c r="BC36"/>
+      <c r="BD36"/>
+      <c r="BE36"/>
+      <c r="BF36"/>
+      <c r="BG36"/>
+      <c r="BH36"/>
+      <c r="BI36"/>
+      <c r="BJ36"/>
+      <c r="BK36"/>
+      <c r="BL36"/>
+    </row>
+    <row r="37" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="58"/>
+      <c r="B37" s="95" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="96" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="97"/>
+      <c r="E37" s="98">
+        <f>F36+1</f>
+        <v>44707</v>
+      </c>
+      <c r="F37" s="98">
+        <f>E37+1</f>
+        <v>44708</v>
+      </c>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="44"/>
+      <c r="K37" s="44"/>
+      <c r="L37" s="44"/>
+      <c r="M37" s="44"/>
+      <c r="N37" s="44"/>
+      <c r="O37" s="44"/>
+      <c r="P37" s="44"/>
+      <c r="Q37" s="44"/>
+      <c r="R37" s="44"/>
+      <c r="S37" s="44"/>
+      <c r="T37" s="44"/>
+      <c r="U37" s="44"/>
+      <c r="V37" s="44"/>
+      <c r="W37" s="44"/>
+      <c r="X37" s="44"/>
+      <c r="Y37" s="44"/>
+      <c r="Z37" s="44"/>
+      <c r="AA37" s="44"/>
+      <c r="AB37" s="44"/>
+      <c r="AC37" s="44"/>
+      <c r="AD37"/>
+      <c r="AE37"/>
+      <c r="AF37"/>
+      <c r="AG37"/>
+      <c r="AH37"/>
+      <c r="AI37"/>
+      <c r="AJ37"/>
+      <c r="AK37"/>
+      <c r="AL37"/>
+      <c r="AM37"/>
+      <c r="AN37"/>
+      <c r="AO37"/>
+      <c r="AP37"/>
+      <c r="AQ37"/>
+      <c r="AR37"/>
+      <c r="AS37"/>
+      <c r="AT37"/>
+      <c r="AU37"/>
+      <c r="AV37"/>
+      <c r="AW37"/>
+      <c r="AX37"/>
+      <c r="AY37"/>
+      <c r="AZ37"/>
+      <c r="BA37"/>
+      <c r="BB37"/>
+      <c r="BC37"/>
+      <c r="BD37"/>
+      <c r="BE37"/>
+      <c r="BF37"/>
+      <c r="BG37"/>
+      <c r="BH37"/>
+      <c r="BI37"/>
+      <c r="BJ37"/>
+      <c r="BK37"/>
+      <c r="BL37"/>
+    </row>
+    <row r="38" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="58"/>
+      <c r="B38" s="95" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="96" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="97"/>
+      <c r="E38" s="98">
+        <f>E35</f>
+        <v>44705</v>
+      </c>
+      <c r="F38" s="98">
+        <f>E38+4</f>
+        <v>44709</v>
+      </c>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17">
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="C34" s="39"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43" t="str">
-        <f t="shared" si="6"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="44"/>
+      <c r="K38" s="44"/>
+      <c r="L38" s="44"/>
+      <c r="M38" s="44"/>
+      <c r="N38" s="44"/>
+      <c r="O38" s="44"/>
+      <c r="P38" s="44"/>
+      <c r="Q38" s="44"/>
+      <c r="R38" s="44"/>
+      <c r="S38" s="44"/>
+      <c r="T38" s="44"/>
+      <c r="U38" s="44"/>
+      <c r="V38" s="44"/>
+      <c r="W38" s="44"/>
+      <c r="X38" s="44"/>
+      <c r="Y38" s="44"/>
+      <c r="Z38" s="44"/>
+      <c r="AA38" s="44"/>
+      <c r="AB38" s="44"/>
+      <c r="AC38" s="44"/>
+      <c r="AD38"/>
+      <c r="AE38"/>
+      <c r="AF38"/>
+      <c r="AG38"/>
+      <c r="AH38"/>
+      <c r="AI38"/>
+      <c r="AJ38"/>
+      <c r="AK38"/>
+      <c r="AL38"/>
+      <c r="AM38"/>
+      <c r="AN38"/>
+      <c r="AO38"/>
+      <c r="AP38"/>
+      <c r="AQ38"/>
+      <c r="AR38"/>
+      <c r="AS38"/>
+      <c r="AT38"/>
+      <c r="AU38"/>
+      <c r="AV38"/>
+      <c r="AW38"/>
+      <c r="AX38"/>
+      <c r="AY38"/>
+      <c r="AZ38"/>
+      <c r="BA38"/>
+      <c r="BB38"/>
+      <c r="BC38"/>
+      <c r="BD38"/>
+      <c r="BE38"/>
+      <c r="BF38"/>
+      <c r="BG38"/>
+      <c r="BH38"/>
+      <c r="BI38"/>
+      <c r="BJ38"/>
+      <c r="BK38"/>
+      <c r="BL38"/>
+    </row>
+    <row r="39" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="79"/>
+      <c r="C39" s="74"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="65"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="I34" s="46"/>
-      <c r="J34" s="46"/>
-      <c r="K34" s="46"/>
-      <c r="L34" s="46"/>
-      <c r="M34" s="46"/>
-      <c r="N34" s="46"/>
-      <c r="O34" s="46"/>
-      <c r="P34" s="46"/>
-      <c r="Q34" s="46"/>
-      <c r="R34" s="46"/>
-      <c r="S34" s="46"/>
-      <c r="T34" s="46"/>
-      <c r="U34" s="46"/>
-      <c r="V34" s="46"/>
-      <c r="W34" s="46"/>
-      <c r="X34" s="46"/>
-      <c r="Y34" s="46"/>
-      <c r="Z34" s="46"/>
-      <c r="AA34" s="46"/>
-      <c r="AB34" s="46"/>
-      <c r="AC34" s="46"/>
-      <c r="AD34" s="46"/>
-      <c r="AE34" s="46"/>
-      <c r="AF34" s="46"/>
-      <c r="AG34" s="46"/>
-      <c r="AH34" s="46"/>
-      <c r="AI34" s="46"/>
-      <c r="AJ34" s="46"/>
-      <c r="AK34" s="46"/>
-      <c r="AL34" s="46"/>
-      <c r="AM34" s="46"/>
-      <c r="AN34" s="46"/>
-      <c r="AO34" s="46"/>
-      <c r="AP34" s="46"/>
-      <c r="AQ34" s="46"/>
-      <c r="AR34" s="46"/>
-      <c r="AS34" s="46"/>
-      <c r="AT34" s="46"/>
-      <c r="AU34" s="46"/>
-      <c r="AV34" s="46"/>
-      <c r="AW34" s="46"/>
-      <c r="AX34" s="46"/>
-      <c r="AY34" s="46"/>
-      <c r="AZ34" s="46"/>
-      <c r="BA34" s="46"/>
-      <c r="BB34" s="46"/>
-      <c r="BC34" s="46"/>
-      <c r="BD34" s="46"/>
-      <c r="BE34" s="46"/>
-      <c r="BF34" s="46"/>
-      <c r="BG34" s="46"/>
-      <c r="BH34" s="46"/>
-      <c r="BI34" s="46"/>
-      <c r="BJ34" s="46"/>
-      <c r="BK34" s="46"/>
-      <c r="BL34" s="46"/>
-    </row>
-    <row r="35" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G35" s="6"/>
-    </row>
-    <row r="36" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="14"/>
-      <c r="F36" s="60"/>
-    </row>
-    <row r="37" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="15"/>
+      <c r="I39" s="44"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="44"/>
+      <c r="L39" s="44"/>
+      <c r="M39" s="44"/>
+      <c r="N39" s="44"/>
+      <c r="O39" s="44"/>
+      <c r="P39" s="44"/>
+      <c r="Q39" s="44"/>
+      <c r="R39" s="44"/>
+      <c r="S39" s="44"/>
+      <c r="T39" s="44"/>
+      <c r="U39" s="44"/>
+      <c r="V39" s="44"/>
+      <c r="W39" s="44"/>
+      <c r="X39" s="44"/>
+      <c r="Y39" s="44"/>
+      <c r="Z39" s="44"/>
+      <c r="AA39" s="44"/>
+      <c r="AB39" s="44"/>
+      <c r="AC39" s="44"/>
+      <c r="AD39"/>
+      <c r="AE39"/>
+      <c r="AF39"/>
+      <c r="AG39"/>
+      <c r="AH39"/>
+      <c r="AI39"/>
+      <c r="AJ39"/>
+      <c r="AK39"/>
+      <c r="AL39"/>
+      <c r="AM39"/>
+      <c r="AN39"/>
+      <c r="AO39"/>
+      <c r="AP39"/>
+      <c r="AQ39"/>
+      <c r="AR39"/>
+      <c r="AS39"/>
+      <c r="AT39"/>
+      <c r="AU39"/>
+      <c r="AV39"/>
+      <c r="AW39"/>
+      <c r="AX39"/>
+      <c r="AY39"/>
+      <c r="AZ39"/>
+      <c r="BA39"/>
+      <c r="BB39"/>
+      <c r="BC39"/>
+      <c r="BD39"/>
+      <c r="BE39"/>
+      <c r="BF39"/>
+      <c r="BG39"/>
+      <c r="BH39"/>
+      <c r="BI39"/>
+      <c r="BJ39"/>
+      <c r="BK39"/>
+      <c r="BL39"/>
+    </row>
+    <row r="40" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="38"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="41"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I40" s="46"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="46"/>
+      <c r="M40" s="46"/>
+      <c r="N40" s="46"/>
+      <c r="O40" s="46"/>
+      <c r="P40" s="46"/>
+      <c r="Q40" s="46"/>
+      <c r="R40" s="46"/>
+      <c r="S40" s="46"/>
+      <c r="T40" s="46"/>
+      <c r="U40" s="46"/>
+      <c r="V40" s="46"/>
+      <c r="W40" s="46"/>
+      <c r="X40" s="46"/>
+      <c r="Y40" s="46"/>
+      <c r="Z40" s="46"/>
+      <c r="AA40" s="46"/>
+      <c r="AB40" s="46"/>
+      <c r="AC40" s="46"/>
+      <c r="AD40"/>
+      <c r="AE40"/>
+      <c r="AF40"/>
+      <c r="AG40"/>
+      <c r="AH40"/>
+      <c r="AI40"/>
+      <c r="AJ40"/>
+      <c r="AK40"/>
+      <c r="AL40"/>
+      <c r="AM40"/>
+      <c r="AN40"/>
+      <c r="AO40"/>
+      <c r="AP40"/>
+      <c r="AQ40"/>
+      <c r="AR40"/>
+      <c r="AS40"/>
+      <c r="AT40"/>
+      <c r="AU40"/>
+      <c r="AV40"/>
+      <c r="AW40"/>
+      <c r="AX40"/>
+      <c r="AY40"/>
+      <c r="AZ40"/>
+      <c r="BA40"/>
+      <c r="BB40"/>
+      <c r="BC40"/>
+      <c r="BD40"/>
+      <c r="BE40"/>
+      <c r="BF40"/>
+      <c r="BG40"/>
+      <c r="BH40"/>
+      <c r="BI40"/>
+      <c r="BJ40"/>
+      <c r="BK40"/>
+      <c r="BL40"/>
+    </row>
+    <row r="41" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G41" s="6"/>
+    </row>
+    <row r="42" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="14"/>
+      <c r="F42" s="60"/>
+    </row>
+    <row r="43" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C43" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="BF4:BL4"/>
+  <mergeCells count="6">
+    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D34">
+  <conditionalFormatting sqref="D7:D40">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4353,12 +4502,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL34">
+  <conditionalFormatting sqref="I5:AC40">
     <cfRule type="expression" dxfId="2" priority="33">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL34">
+  <conditionalFormatting sqref="I7:AC40">
     <cfRule type="expression" dxfId="1" priority="27">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4371,13 +4520,9 @@
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="I1" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-  </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="57" fitToHeight="0" orientation="landscape" r:id="rId3"/>
+  <pageSetup scale="57" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -4397,7 +4542,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D34</xm:sqref>
+          <xm:sqref>D7:D40</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4420,79 +4565,79 @@
     <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:2" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B2" s="49"/>
     </row>
     <row r="3" spans="1:2" s="54" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="83" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B3" s="55"/>
     </row>
     <row r="4" spans="1:2" s="51" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A4" s="52" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="53" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="52" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="48" customFormat="1" ht="204.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="57" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="51" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A8" s="52" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.2">
       <c r="A9" s="53" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="48" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="56" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="51" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A11" s="52" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="53" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="48" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="56" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="51" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A14" s="52" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="53" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="75" x14ac:dyDescent="0.2">
       <c r="A16" s="53" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>